<commit_message>
adding more return objs
</commit_message>
<xml_diff>
--- a/refined_divisions/test_19.xlsx
+++ b/refined_divisions/test_19.xlsx
@@ -244,6 +244,27 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -256,6 +277,15 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -268,6 +298,24 @@
     <xf numFmtId="0" fontId="3" fillId="3" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -294,54 +342,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="3" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="11" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -739,8 +739,8 @@
   </sheetPr>
   <dimension ref="A1:S128"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="V43" sqref="V43"/>
+    <sheetView tabSelected="1" topLeftCell="A79" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="Q89" sqref="Q89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
@@ -752,27 +752,27 @@
   </cols>
   <sheetData>
     <row r="1" ht="8.1" customHeight="1" s="18">
-      <c r="B1" s="51" t="inlineStr">
+      <c r="B1" s="37" t="inlineStr">
         <is>
           <t>Round of 32</t>
         </is>
       </c>
-      <c r="E1" s="51" t="inlineStr">
+      <c r="E1" s="37" t="inlineStr">
         <is>
           <t>Round of 16</t>
         </is>
       </c>
-      <c r="H1" s="51" t="inlineStr">
+      <c r="H1" s="37" t="inlineStr">
         <is>
           <t>Quarter-Final</t>
         </is>
       </c>
-      <c r="K1" s="51" t="inlineStr">
+      <c r="K1" s="37" t="inlineStr">
         <is>
           <t>Semi-Final</t>
         </is>
       </c>
-      <c r="N1" s="51" t="inlineStr">
+      <c r="N1" s="37" t="inlineStr">
         <is>
           <t>Final</t>
         </is>
@@ -807,15 +807,15 @@
       <c r="C4" s="62" t="n"/>
     </row>
     <row r="5" ht="8.1" customHeight="1" s="18">
-      <c r="B5" s="55" t="n"/>
-      <c r="C5" s="55" t="n"/>
+      <c r="B5" s="27" t="n"/>
+      <c r="C5" s="27" t="n"/>
       <c r="D5" s="22" t="n"/>
       <c r="E5" s="59" t="inlineStr"/>
       <c r="F5" s="60" t="n"/>
     </row>
     <row r="6" ht="8.1" customHeight="1" s="18">
-      <c r="B6" s="55" t="n"/>
-      <c r="C6" s="55" t="n"/>
+      <c r="B6" s="27" t="n"/>
+      <c r="C6" s="27" t="n"/>
       <c r="D6" s="19" t="n"/>
       <c r="E6" s="61" t="inlineStr"/>
       <c r="F6" s="62" t="n"/>
@@ -838,8 +838,8 @@
         </is>
       </c>
       <c r="C7" s="60" t="n"/>
-      <c r="E7" s="55" t="n"/>
-      <c r="F7" s="55" t="n"/>
+      <c r="E7" s="27" t="n"/>
+      <c r="F7" s="27" t="n"/>
       <c r="G7" s="20" t="n"/>
       <c r="K7" s="20" t="n"/>
       <c r="Q7" s="66" t="n"/>
@@ -851,17 +851,17 @@
         </is>
       </c>
       <c r="C8" s="62" t="n"/>
-      <c r="E8" s="55" t="n"/>
-      <c r="F8" s="55" t="n"/>
+      <c r="E8" s="27" t="n"/>
+      <c r="F8" s="27" t="n"/>
       <c r="G8" s="20" t="n"/>
       <c r="K8" s="20" t="n"/>
       <c r="Q8" s="66" t="n"/>
     </row>
     <row r="9" ht="8.1" customHeight="1" s="18">
-      <c r="B9" s="55" t="n"/>
-      <c r="C9" s="55" t="n"/>
-      <c r="E9" s="55" t="n"/>
-      <c r="F9" s="55" t="n"/>
+      <c r="B9" s="27" t="n"/>
+      <c r="C9" s="27" t="n"/>
+      <c r="E9" s="27" t="n"/>
+      <c r="F9" s="27" t="n"/>
       <c r="G9" s="22" t="n"/>
       <c r="H9" s="59" t="n"/>
       <c r="I9" s="60" t="n"/>
@@ -874,10 +874,10 @@
       <c r="Q9" s="62" t="n"/>
     </row>
     <row r="10" ht="8.1" customHeight="1" s="18">
-      <c r="B10" s="55" t="n"/>
-      <c r="C10" s="55" t="n"/>
-      <c r="E10" s="55" t="n"/>
-      <c r="F10" s="55" t="n"/>
+      <c r="B10" s="27" t="n"/>
+      <c r="C10" s="27" t="n"/>
+      <c r="E10" s="27" t="n"/>
+      <c r="F10" s="27" t="n"/>
       <c r="G10" s="20" t="n"/>
       <c r="H10" s="61" t="n"/>
       <c r="I10" s="62" t="n"/>
@@ -889,26 +889,26 @@
         </is>
       </c>
       <c r="C11" s="60" t="n"/>
-      <c r="E11" s="55" t="n"/>
-      <c r="F11" s="55" t="n"/>
+      <c r="E11" s="27" t="n"/>
+      <c r="F11" s="27" t="n"/>
       <c r="G11" s="20" t="n"/>
-      <c r="H11" s="55" t="n"/>
-      <c r="I11" s="55" t="n"/>
+      <c r="H11" s="27" t="n"/>
+      <c r="I11" s="27" t="n"/>
       <c r="J11" s="20" t="n"/>
     </row>
     <row r="12" ht="8.1" customHeight="1" s="18">
       <c r="B12" s="61" t="inlineStr"/>
       <c r="C12" s="62" t="n"/>
-      <c r="E12" s="55" t="n"/>
-      <c r="F12" s="55" t="n"/>
+      <c r="E12" s="27" t="n"/>
+      <c r="F12" s="27" t="n"/>
       <c r="G12" s="20" t="n"/>
-      <c r="H12" s="55" t="n"/>
-      <c r="I12" s="55" t="n"/>
+      <c r="H12" s="27" t="n"/>
+      <c r="I12" s="27" t="n"/>
       <c r="J12" s="20" t="n"/>
     </row>
     <row r="13" ht="8.1" customHeight="1" s="18">
-      <c r="B13" s="55" t="n"/>
-      <c r="C13" s="55" t="n"/>
+      <c r="B13" s="27" t="n"/>
+      <c r="C13" s="27" t="n"/>
       <c r="D13" s="22" t="n"/>
       <c r="E13" s="65" t="inlineStr">
         <is>
@@ -916,13 +916,13 @@
         </is>
       </c>
       <c r="F13" s="60" t="n"/>
-      <c r="H13" s="55" t="n"/>
-      <c r="I13" s="55" t="n"/>
+      <c r="H13" s="27" t="n"/>
+      <c r="I13" s="27" t="n"/>
       <c r="J13" s="20" t="n"/>
     </row>
     <row r="14" ht="8.1" customHeight="1" s="18">
-      <c r="B14" s="55" t="n"/>
-      <c r="C14" s="55" t="n"/>
+      <c r="B14" s="27" t="n"/>
+      <c r="C14" s="27" t="n"/>
       <c r="D14" s="19" t="n"/>
       <c r="E14" s="67" t="inlineStr">
         <is>
@@ -930,8 +930,8 @@
         </is>
       </c>
       <c r="F14" s="62" t="n"/>
-      <c r="H14" s="55" t="n"/>
-      <c r="I14" s="55" t="n"/>
+      <c r="H14" s="27" t="n"/>
+      <c r="I14" s="27" t="n"/>
       <c r="J14" s="20" t="n"/>
     </row>
     <row r="15" ht="8.1" customHeight="1" s="18">
@@ -941,10 +941,10 @@
         </is>
       </c>
       <c r="C15" s="60" t="n"/>
-      <c r="E15" s="55" t="n"/>
-      <c r="F15" s="55" t="n"/>
-      <c r="H15" s="55" t="n"/>
-      <c r="I15" s="55" t="n"/>
+      <c r="E15" s="27" t="n"/>
+      <c r="F15" s="27" t="n"/>
+      <c r="H15" s="27" t="n"/>
+      <c r="I15" s="27" t="n"/>
       <c r="J15" s="20" t="n"/>
     </row>
     <row r="16" ht="8.1" customHeight="1" s="18">
@@ -954,30 +954,30 @@
         </is>
       </c>
       <c r="C16" s="62" t="n"/>
-      <c r="E16" s="55" t="n"/>
-      <c r="F16" s="55" t="n"/>
-      <c r="H16" s="55" t="n"/>
-      <c r="I16" s="55" t="n"/>
+      <c r="E16" s="27" t="n"/>
+      <c r="F16" s="27" t="n"/>
+      <c r="H16" s="27" t="n"/>
+      <c r="I16" s="27" t="n"/>
       <c r="J16" s="20" t="n"/>
     </row>
     <row r="17" ht="8.1" customHeight="1" s="18">
-      <c r="B17" s="55" t="n"/>
-      <c r="C17" s="55" t="n"/>
-      <c r="E17" s="55" t="n"/>
-      <c r="F17" s="55" t="n"/>
-      <c r="H17" s="55" t="n"/>
-      <c r="I17" s="55" t="n"/>
+      <c r="B17" s="27" t="n"/>
+      <c r="C17" s="27" t="n"/>
+      <c r="E17" s="27" t="n"/>
+      <c r="F17" s="27" t="n"/>
+      <c r="H17" s="27" t="n"/>
+      <c r="I17" s="27" t="n"/>
       <c r="J17" s="22" t="n"/>
       <c r="K17" s="59" t="n"/>
       <c r="L17" s="60" t="n"/>
     </row>
     <row r="18" ht="8.1" customHeight="1" s="18">
-      <c r="B18" s="55" t="n"/>
-      <c r="C18" s="55" t="n"/>
-      <c r="E18" s="55" t="n"/>
-      <c r="F18" s="55" t="n"/>
-      <c r="H18" s="55" t="n"/>
-      <c r="I18" s="55" t="n"/>
+      <c r="B18" s="27" t="n"/>
+      <c r="C18" s="27" t="n"/>
+      <c r="E18" s="27" t="n"/>
+      <c r="F18" s="27" t="n"/>
+      <c r="H18" s="27" t="n"/>
+      <c r="I18" s="27" t="n"/>
       <c r="J18" s="20" t="n"/>
       <c r="K18" s="61" t="n"/>
       <c r="L18" s="62" t="n"/>
@@ -989,13 +989,13 @@
         </is>
       </c>
       <c r="C19" s="60" t="n"/>
-      <c r="E19" s="55" t="n"/>
-      <c r="F19" s="55" t="n"/>
-      <c r="H19" s="55" t="n"/>
-      <c r="I19" s="55" t="n"/>
+      <c r="E19" s="27" t="n"/>
+      <c r="F19" s="27" t="n"/>
+      <c r="H19" s="27" t="n"/>
+      <c r="I19" s="27" t="n"/>
       <c r="J19" s="20" t="n"/>
-      <c r="K19" s="55" t="n"/>
-      <c r="L19" s="55" t="n"/>
+      <c r="K19" s="27" t="n"/>
+      <c r="L19" s="27" t="n"/>
       <c r="M19" s="20" t="n"/>
     </row>
     <row r="20" ht="8.1" customHeight="1" s="18">
@@ -1005,18 +1005,18 @@
         </is>
       </c>
       <c r="C20" s="62" t="n"/>
-      <c r="E20" s="55" t="n"/>
-      <c r="F20" s="55" t="n"/>
-      <c r="H20" s="55" t="n"/>
-      <c r="I20" s="55" t="n"/>
+      <c r="E20" s="27" t="n"/>
+      <c r="F20" s="27" t="n"/>
+      <c r="H20" s="27" t="n"/>
+      <c r="I20" s="27" t="n"/>
       <c r="J20" s="20" t="n"/>
-      <c r="K20" s="55" t="n"/>
-      <c r="L20" s="55" t="n"/>
+      <c r="K20" s="27" t="n"/>
+      <c r="L20" s="27" t="n"/>
       <c r="M20" s="20" t="n"/>
     </row>
     <row r="21" ht="8.1" customHeight="1" s="18">
-      <c r="B21" s="55" t="n"/>
-      <c r="C21" s="55" t="n"/>
+      <c r="B21" s="27" t="n"/>
+      <c r="C21" s="27" t="n"/>
       <c r="D21" s="22" t="n"/>
       <c r="E21" s="59" t="inlineStr">
         <is>
@@ -1024,16 +1024,16 @@
         </is>
       </c>
       <c r="F21" s="60" t="n"/>
-      <c r="H21" s="55" t="n"/>
-      <c r="I21" s="55" t="n"/>
+      <c r="H21" s="27" t="n"/>
+      <c r="I21" s="27" t="n"/>
       <c r="J21" s="20" t="n"/>
-      <c r="K21" s="55" t="n"/>
-      <c r="L21" s="55" t="n"/>
+      <c r="K21" s="27" t="n"/>
+      <c r="L21" s="27" t="n"/>
       <c r="M21" s="20" t="n"/>
     </row>
     <row r="22" ht="8.1" customHeight="1" s="18">
-      <c r="B22" s="55" t="n"/>
-      <c r="C22" s="55" t="n"/>
+      <c r="B22" s="27" t="n"/>
+      <c r="C22" s="27" t="n"/>
       <c r="D22" s="19" t="n"/>
       <c r="E22" s="61" t="inlineStr">
         <is>
@@ -1041,11 +1041,11 @@
         </is>
       </c>
       <c r="F22" s="62" t="n"/>
-      <c r="H22" s="55" t="n"/>
-      <c r="I22" s="55" t="n"/>
+      <c r="H22" s="27" t="n"/>
+      <c r="I22" s="27" t="n"/>
       <c r="J22" s="20" t="n"/>
-      <c r="K22" s="55" t="n"/>
-      <c r="L22" s="55" t="n"/>
+      <c r="K22" s="27" t="n"/>
+      <c r="L22" s="27" t="n"/>
       <c r="M22" s="20" t="n"/>
     </row>
     <row r="23" ht="8.1" customHeight="1" s="18">
@@ -1055,51 +1055,51 @@
         </is>
       </c>
       <c r="C23" s="60" t="n"/>
-      <c r="E23" s="55" t="n"/>
-      <c r="F23" s="55" t="n"/>
+      <c r="E23" s="27" t="n"/>
+      <c r="F23" s="27" t="n"/>
       <c r="G23" s="20" t="n"/>
-      <c r="H23" s="55" t="n"/>
-      <c r="I23" s="55" t="n"/>
+      <c r="H23" s="27" t="n"/>
+      <c r="I23" s="27" t="n"/>
       <c r="J23" s="20" t="n"/>
-      <c r="K23" s="55" t="n"/>
-      <c r="L23" s="55" t="n"/>
+      <c r="K23" s="27" t="n"/>
+      <c r="L23" s="27" t="n"/>
       <c r="M23" s="20" t="n"/>
     </row>
     <row r="24" ht="8.1" customHeight="1" s="18">
       <c r="B24" s="67" t="inlineStr"/>
       <c r="C24" s="62" t="n"/>
-      <c r="E24" s="55" t="n"/>
-      <c r="F24" s="55" t="n"/>
+      <c r="E24" s="27" t="n"/>
+      <c r="F24" s="27" t="n"/>
       <c r="G24" s="20" t="n"/>
-      <c r="H24" s="55" t="n"/>
-      <c r="I24" s="55" t="n"/>
+      <c r="H24" s="27" t="n"/>
+      <c r="I24" s="27" t="n"/>
       <c r="J24" s="20" t="n"/>
-      <c r="K24" s="55" t="n"/>
-      <c r="L24" s="55" t="n"/>
+      <c r="K24" s="27" t="n"/>
+      <c r="L24" s="27" t="n"/>
       <c r="M24" s="20" t="n"/>
     </row>
     <row r="25" ht="8.1" customHeight="1" s="18">
-      <c r="B25" s="55" t="n"/>
-      <c r="C25" s="55" t="n"/>
-      <c r="E25" s="55" t="n"/>
-      <c r="F25" s="55" t="n"/>
+      <c r="B25" s="27" t="n"/>
+      <c r="C25" s="27" t="n"/>
+      <c r="E25" s="27" t="n"/>
+      <c r="F25" s="27" t="n"/>
       <c r="G25" s="22" t="n"/>
       <c r="H25" s="65" t="n"/>
       <c r="I25" s="60" t="n"/>
-      <c r="K25" s="55" t="n"/>
-      <c r="L25" s="55" t="n"/>
+      <c r="K25" s="27" t="n"/>
+      <c r="L25" s="27" t="n"/>
       <c r="M25" s="20" t="n"/>
     </row>
     <row r="26" ht="8.1" customHeight="1" s="18">
-      <c r="B26" s="55" t="n"/>
-      <c r="C26" s="55" t="n"/>
-      <c r="E26" s="55" t="n"/>
-      <c r="F26" s="55" t="n"/>
+      <c r="B26" s="27" t="n"/>
+      <c r="C26" s="27" t="n"/>
+      <c r="E26" s="27" t="n"/>
+      <c r="F26" s="27" t="n"/>
       <c r="G26" s="20" t="n"/>
       <c r="H26" s="67" t="n"/>
       <c r="I26" s="62" t="n"/>
-      <c r="K26" s="55" t="n"/>
-      <c r="L26" s="55" t="n"/>
+      <c r="K26" s="27" t="n"/>
+      <c r="L26" s="27" t="n"/>
       <c r="M26" s="20" t="n"/>
     </row>
     <row r="27" ht="8.1" customHeight="1" s="18">
@@ -1109,30 +1109,30 @@
         </is>
       </c>
       <c r="C27" s="60" t="n"/>
-      <c r="E27" s="55" t="n"/>
-      <c r="F27" s="55" t="n"/>
+      <c r="E27" s="27" t="n"/>
+      <c r="F27" s="27" t="n"/>
       <c r="G27" s="20" t="n"/>
-      <c r="H27" s="55" t="n"/>
-      <c r="I27" s="55" t="n"/>
-      <c r="K27" s="55" t="n"/>
-      <c r="L27" s="55" t="n"/>
+      <c r="H27" s="27" t="n"/>
+      <c r="I27" s="27" t="n"/>
+      <c r="K27" s="27" t="n"/>
+      <c r="L27" s="27" t="n"/>
       <c r="M27" s="20" t="n"/>
     </row>
     <row r="28" ht="8.1" customHeight="1" s="18">
       <c r="B28" s="61" t="inlineStr"/>
       <c r="C28" s="62" t="n"/>
-      <c r="E28" s="55" t="n"/>
-      <c r="F28" s="55" t="n"/>
+      <c r="E28" s="27" t="n"/>
+      <c r="F28" s="27" t="n"/>
       <c r="G28" s="20" t="n"/>
-      <c r="H28" s="55" t="n"/>
-      <c r="I28" s="55" t="n"/>
-      <c r="K28" s="55" t="n"/>
-      <c r="L28" s="55" t="n"/>
+      <c r="H28" s="27" t="n"/>
+      <c r="I28" s="27" t="n"/>
+      <c r="K28" s="27" t="n"/>
+      <c r="L28" s="27" t="n"/>
       <c r="M28" s="20" t="n"/>
     </row>
     <row r="29" ht="8.1" customHeight="1" s="18">
-      <c r="B29" s="55" t="n"/>
-      <c r="C29" s="55" t="n"/>
+      <c r="B29" s="27" t="n"/>
+      <c r="C29" s="27" t="n"/>
       <c r="D29" s="22" t="n"/>
       <c r="E29" s="65" t="inlineStr">
         <is>
@@ -1140,15 +1140,15 @@
         </is>
       </c>
       <c r="F29" s="60" t="n"/>
-      <c r="H29" s="55" t="n"/>
-      <c r="I29" s="55" t="n"/>
-      <c r="K29" s="55" t="n"/>
-      <c r="L29" s="55" t="n"/>
+      <c r="H29" s="27" t="n"/>
+      <c r="I29" s="27" t="n"/>
+      <c r="K29" s="27" t="n"/>
+      <c r="L29" s="27" t="n"/>
       <c r="M29" s="20" t="n"/>
     </row>
     <row r="30" ht="8.1" customHeight="1" s="18">
-      <c r="B30" s="55" t="n"/>
-      <c r="C30" s="55" t="n"/>
+      <c r="B30" s="27" t="n"/>
+      <c r="C30" s="27" t="n"/>
       <c r="D30" s="19" t="n"/>
       <c r="E30" s="67" t="inlineStr">
         <is>
@@ -1156,10 +1156,10 @@
         </is>
       </c>
       <c r="F30" s="62" t="n"/>
-      <c r="H30" s="55" t="n"/>
-      <c r="I30" s="55" t="n"/>
-      <c r="K30" s="55" t="n"/>
-      <c r="L30" s="55" t="n"/>
+      <c r="H30" s="27" t="n"/>
+      <c r="I30" s="27" t="n"/>
+      <c r="K30" s="27" t="n"/>
+      <c r="L30" s="27" t="n"/>
       <c r="M30" s="20" t="n"/>
     </row>
     <row r="31" ht="8.1" customHeight="1" s="18">
@@ -1169,12 +1169,12 @@
         </is>
       </c>
       <c r="C31" s="60" t="n"/>
-      <c r="E31" s="55" t="n"/>
-      <c r="F31" s="55" t="n"/>
-      <c r="H31" s="55" t="n"/>
-      <c r="I31" s="55" t="n"/>
-      <c r="K31" s="55" t="n"/>
-      <c r="L31" s="55" t="n"/>
+      <c r="E31" s="27" t="n"/>
+      <c r="F31" s="27" t="n"/>
+      <c r="H31" s="27" t="n"/>
+      <c r="I31" s="27" t="n"/>
+      <c r="K31" s="27" t="n"/>
+      <c r="L31" s="27" t="n"/>
       <c r="M31" s="20" t="n"/>
     </row>
     <row r="32" ht="8.1" customHeight="1" s="18">
@@ -1184,36 +1184,36 @@
         </is>
       </c>
       <c r="C32" s="62" t="n"/>
-      <c r="E32" s="55" t="n"/>
-      <c r="F32" s="55" t="n"/>
-      <c r="H32" s="55" t="n"/>
-      <c r="I32" s="55" t="n"/>
-      <c r="K32" s="55" t="n"/>
-      <c r="L32" s="55" t="n"/>
+      <c r="E32" s="27" t="n"/>
+      <c r="F32" s="27" t="n"/>
+      <c r="H32" s="27" t="n"/>
+      <c r="I32" s="27" t="n"/>
+      <c r="K32" s="27" t="n"/>
+      <c r="L32" s="27" t="n"/>
       <c r="M32" s="20" t="n"/>
     </row>
     <row r="33" ht="8.1" customHeight="1" s="18">
-      <c r="B33" s="55" t="n"/>
-      <c r="C33" s="55" t="n"/>
-      <c r="E33" s="55" t="n"/>
-      <c r="F33" s="55" t="n"/>
-      <c r="H33" s="55" t="n"/>
-      <c r="I33" s="55" t="n"/>
-      <c r="K33" s="55" t="n"/>
-      <c r="L33" s="55" t="n"/>
+      <c r="B33" s="27" t="n"/>
+      <c r="C33" s="27" t="n"/>
+      <c r="E33" s="27" t="n"/>
+      <c r="F33" s="27" t="n"/>
+      <c r="H33" s="27" t="n"/>
+      <c r="I33" s="27" t="n"/>
+      <c r="K33" s="27" t="n"/>
+      <c r="L33" s="27" t="n"/>
       <c r="M33" s="22" t="n"/>
       <c r="N33" s="59" t="n"/>
       <c r="O33" s="60" t="n"/>
     </row>
     <row r="34" ht="8.1" customHeight="1" s="18">
-      <c r="B34" s="55" t="n"/>
-      <c r="C34" s="55" t="n"/>
-      <c r="E34" s="55" t="n"/>
-      <c r="F34" s="55" t="n"/>
-      <c r="H34" s="55" t="n"/>
-      <c r="I34" s="55" t="n"/>
-      <c r="K34" s="55" t="n"/>
-      <c r="L34" s="55" t="n"/>
+      <c r="B34" s="27" t="n"/>
+      <c r="C34" s="27" t="n"/>
+      <c r="E34" s="27" t="n"/>
+      <c r="F34" s="27" t="n"/>
+      <c r="H34" s="27" t="n"/>
+      <c r="I34" s="27" t="n"/>
+      <c r="K34" s="27" t="n"/>
+      <c r="L34" s="27" t="n"/>
       <c r="M34" s="20" t="n"/>
       <c r="N34" s="61" t="n"/>
       <c r="O34" s="62" t="n"/>
@@ -1225,15 +1225,15 @@
         </is>
       </c>
       <c r="C35" s="60" t="n"/>
-      <c r="E35" s="55" t="n"/>
-      <c r="F35" s="55" t="n"/>
-      <c r="H35" s="55" t="n"/>
-      <c r="I35" s="55" t="n"/>
-      <c r="K35" s="55" t="n"/>
-      <c r="L35" s="55" t="n"/>
+      <c r="E35" s="27" t="n"/>
+      <c r="F35" s="27" t="n"/>
+      <c r="H35" s="27" t="n"/>
+      <c r="I35" s="27" t="n"/>
+      <c r="K35" s="27" t="n"/>
+      <c r="L35" s="27" t="n"/>
       <c r="M35" s="20" t="n"/>
-      <c r="N35" s="55" t="n"/>
-      <c r="O35" s="53" t="n"/>
+      <c r="N35" s="27" t="n"/>
+      <c r="O35" s="25" t="n"/>
     </row>
     <row r="36" ht="8.1" customHeight="1" s="18">
       <c r="B36" s="61" t="inlineStr">
@@ -1242,19 +1242,19 @@
         </is>
       </c>
       <c r="C36" s="62" t="n"/>
-      <c r="E36" s="55" t="n"/>
-      <c r="F36" s="55" t="n"/>
-      <c r="H36" s="55" t="n"/>
-      <c r="I36" s="55" t="n"/>
-      <c r="K36" s="55" t="n"/>
-      <c r="L36" s="55" t="n"/>
+      <c r="E36" s="27" t="n"/>
+      <c r="F36" s="27" t="n"/>
+      <c r="H36" s="27" t="n"/>
+      <c r="I36" s="27" t="n"/>
+      <c r="K36" s="27" t="n"/>
+      <c r="L36" s="27" t="n"/>
       <c r="M36" s="20" t="n"/>
-      <c r="N36" s="55" t="n"/>
-      <c r="O36" s="54" t="n"/>
+      <c r="N36" s="27" t="n"/>
+      <c r="O36" s="26" t="n"/>
     </row>
     <row r="37" ht="8.1" customHeight="1" s="18">
-      <c r="B37" s="55" t="n"/>
-      <c r="C37" s="55" t="n"/>
+      <c r="B37" s="27" t="n"/>
+      <c r="C37" s="27" t="n"/>
       <c r="D37" s="22" t="n"/>
       <c r="E37" s="59" t="inlineStr">
         <is>
@@ -1262,17 +1262,17 @@
         </is>
       </c>
       <c r="F37" s="60" t="n"/>
-      <c r="H37" s="55" t="n"/>
-      <c r="I37" s="55" t="n"/>
-      <c r="K37" s="55" t="n"/>
-      <c r="L37" s="55" t="n"/>
+      <c r="H37" s="27" t="n"/>
+      <c r="I37" s="27" t="n"/>
+      <c r="K37" s="27" t="n"/>
+      <c r="L37" s="27" t="n"/>
       <c r="M37" s="20" t="n"/>
-      <c r="N37" s="55" t="n"/>
-      <c r="O37" s="54" t="n"/>
+      <c r="N37" s="27" t="n"/>
+      <c r="O37" s="26" t="n"/>
     </row>
     <row r="38" ht="8.1" customHeight="1" s="18">
-      <c r="B38" s="55" t="n"/>
-      <c r="C38" s="55" t="n"/>
+      <c r="B38" s="27" t="n"/>
+      <c r="C38" s="27" t="n"/>
       <c r="D38" s="19" t="n"/>
       <c r="E38" s="61" t="inlineStr">
         <is>
@@ -1280,13 +1280,13 @@
         </is>
       </c>
       <c r="F38" s="62" t="n"/>
-      <c r="H38" s="55" t="n"/>
-      <c r="I38" s="55" t="n"/>
-      <c r="K38" s="55" t="n"/>
-      <c r="L38" s="55" t="n"/>
+      <c r="H38" s="27" t="n"/>
+      <c r="I38" s="27" t="n"/>
+      <c r="K38" s="27" t="n"/>
+      <c r="L38" s="27" t="n"/>
       <c r="M38" s="20" t="n"/>
-      <c r="N38" s="55" t="n"/>
-      <c r="O38" s="54" t="n"/>
+      <c r="N38" s="27" t="n"/>
+      <c r="O38" s="26" t="n"/>
     </row>
     <row r="39" ht="8.1" customHeight="1" s="18">
       <c r="B39" s="65" t="inlineStr">
@@ -1295,58 +1295,58 @@
         </is>
       </c>
       <c r="C39" s="60" t="n"/>
-      <c r="E39" s="55" t="n"/>
-      <c r="F39" s="55" t="n"/>
+      <c r="E39" s="27" t="n"/>
+      <c r="F39" s="27" t="n"/>
       <c r="G39" s="20" t="n"/>
-      <c r="H39" s="55" t="n"/>
-      <c r="I39" s="55" t="n"/>
-      <c r="K39" s="55" t="n"/>
-      <c r="L39" s="55" t="n"/>
+      <c r="H39" s="27" t="n"/>
+      <c r="I39" s="27" t="n"/>
+      <c r="K39" s="27" t="n"/>
+      <c r="L39" s="27" t="n"/>
       <c r="M39" s="20" t="n"/>
-      <c r="N39" s="55" t="n"/>
-      <c r="O39" s="54" t="n"/>
+      <c r="N39" s="27" t="n"/>
+      <c r="O39" s="26" t="n"/>
     </row>
     <row r="40" ht="8.1" customHeight="1" s="18">
       <c r="B40" s="67" t="inlineStr"/>
       <c r="C40" s="62" t="n"/>
-      <c r="E40" s="55" t="n"/>
-      <c r="F40" s="55" t="n"/>
+      <c r="E40" s="27" t="n"/>
+      <c r="F40" s="27" t="n"/>
       <c r="G40" s="20" t="n"/>
-      <c r="H40" s="55" t="n"/>
-      <c r="I40" s="55" t="n"/>
-      <c r="K40" s="55" t="n"/>
-      <c r="L40" s="55" t="n"/>
+      <c r="H40" s="27" t="n"/>
+      <c r="I40" s="27" t="n"/>
+      <c r="K40" s="27" t="n"/>
+      <c r="L40" s="27" t="n"/>
       <c r="M40" s="20" t="n"/>
-      <c r="N40" s="55" t="n"/>
-      <c r="O40" s="54" t="n"/>
+      <c r="N40" s="27" t="n"/>
+      <c r="O40" s="26" t="n"/>
     </row>
     <row r="41" ht="8.1" customHeight="1" s="18">
-      <c r="B41" s="55" t="n"/>
-      <c r="C41" s="55" t="n"/>
-      <c r="E41" s="55" t="n"/>
-      <c r="F41" s="55" t="n"/>
+      <c r="B41" s="27" t="n"/>
+      <c r="C41" s="27" t="n"/>
+      <c r="E41" s="27" t="n"/>
+      <c r="F41" s="27" t="n"/>
       <c r="G41" s="22" t="n"/>
       <c r="H41" s="59" t="n"/>
       <c r="I41" s="60" t="n"/>
-      <c r="K41" s="55" t="n"/>
-      <c r="L41" s="55" t="n"/>
+      <c r="K41" s="27" t="n"/>
+      <c r="L41" s="27" t="n"/>
       <c r="M41" s="20" t="n"/>
-      <c r="N41" s="55" t="n"/>
-      <c r="O41" s="54" t="n"/>
+      <c r="N41" s="27" t="n"/>
+      <c r="O41" s="26" t="n"/>
     </row>
     <row r="42" ht="8.1" customHeight="1" s="18">
-      <c r="B42" s="55" t="n"/>
-      <c r="C42" s="55" t="n"/>
-      <c r="E42" s="55" t="n"/>
-      <c r="F42" s="55" t="n"/>
+      <c r="B42" s="27" t="n"/>
+      <c r="C42" s="27" t="n"/>
+      <c r="E42" s="27" t="n"/>
+      <c r="F42" s="27" t="n"/>
       <c r="G42" s="20" t="n"/>
       <c r="H42" s="61" t="n"/>
       <c r="I42" s="62" t="n"/>
-      <c r="K42" s="55" t="n"/>
-      <c r="L42" s="55" t="n"/>
+      <c r="K42" s="27" t="n"/>
+      <c r="L42" s="27" t="n"/>
       <c r="M42" s="20" t="n"/>
-      <c r="N42" s="55" t="n"/>
-      <c r="O42" s="54" t="n"/>
+      <c r="N42" s="27" t="n"/>
+      <c r="O42" s="26" t="n"/>
     </row>
     <row r="43" ht="8.1" customHeight="1" s="18">
       <c r="B43" s="59" t="inlineStr">
@@ -1355,36 +1355,36 @@
         </is>
       </c>
       <c r="C43" s="60" t="n"/>
-      <c r="E43" s="55" t="n"/>
-      <c r="F43" s="55" t="n"/>
+      <c r="E43" s="27" t="n"/>
+      <c r="F43" s="27" t="n"/>
       <c r="G43" s="20" t="n"/>
-      <c r="H43" s="55" t="n"/>
-      <c r="I43" s="55" t="n"/>
+      <c r="H43" s="27" t="n"/>
+      <c r="I43" s="27" t="n"/>
       <c r="J43" s="20" t="n"/>
-      <c r="K43" s="55" t="n"/>
-      <c r="L43" s="55" t="n"/>
+      <c r="K43" s="27" t="n"/>
+      <c r="L43" s="27" t="n"/>
       <c r="M43" s="20" t="n"/>
-      <c r="N43" s="55" t="n"/>
-      <c r="O43" s="54" t="n"/>
+      <c r="N43" s="27" t="n"/>
+      <c r="O43" s="26" t="n"/>
     </row>
     <row r="44" ht="8.1" customHeight="1" s="18">
       <c r="B44" s="61" t="inlineStr"/>
       <c r="C44" s="62" t="n"/>
-      <c r="E44" s="55" t="n"/>
-      <c r="F44" s="55" t="n"/>
+      <c r="E44" s="27" t="n"/>
+      <c r="F44" s="27" t="n"/>
       <c r="G44" s="20" t="n"/>
-      <c r="H44" s="55" t="n"/>
-      <c r="I44" s="55" t="n"/>
+      <c r="H44" s="27" t="n"/>
+      <c r="I44" s="27" t="n"/>
       <c r="J44" s="20" t="n"/>
-      <c r="K44" s="55" t="n"/>
-      <c r="L44" s="55" t="n"/>
+      <c r="K44" s="27" t="n"/>
+      <c r="L44" s="27" t="n"/>
       <c r="M44" s="20" t="n"/>
-      <c r="N44" s="55" t="n"/>
-      <c r="O44" s="54" t="n"/>
+      <c r="N44" s="27" t="n"/>
+      <c r="O44" s="26" t="n"/>
     </row>
     <row r="45" ht="8.1" customHeight="1" s="18">
-      <c r="B45" s="55" t="n"/>
-      <c r="C45" s="55" t="n"/>
+      <c r="B45" s="27" t="n"/>
+      <c r="C45" s="27" t="n"/>
       <c r="D45" s="22" t="n"/>
       <c r="E45" s="65" t="inlineStr">
         <is>
@@ -1392,18 +1392,18 @@
         </is>
       </c>
       <c r="F45" s="60" t="n"/>
-      <c r="H45" s="55" t="n"/>
-      <c r="I45" s="55" t="n"/>
+      <c r="H45" s="27" t="n"/>
+      <c r="I45" s="27" t="n"/>
       <c r="J45" s="20" t="n"/>
-      <c r="K45" s="55" t="n"/>
-      <c r="L45" s="55" t="n"/>
+      <c r="K45" s="27" t="n"/>
+      <c r="L45" s="27" t="n"/>
       <c r="M45" s="20" t="n"/>
-      <c r="N45" s="55" t="n"/>
-      <c r="O45" s="54" t="n"/>
+      <c r="N45" s="27" t="n"/>
+      <c r="O45" s="26" t="n"/>
     </row>
     <row r="46" ht="8.1" customHeight="1" s="18">
-      <c r="B46" s="55" t="n"/>
-      <c r="C46" s="55" t="n"/>
+      <c r="B46" s="27" t="n"/>
+      <c r="C46" s="27" t="n"/>
       <c r="D46" s="19" t="n"/>
       <c r="E46" s="67" t="inlineStr">
         <is>
@@ -1411,14 +1411,14 @@
         </is>
       </c>
       <c r="F46" s="62" t="n"/>
-      <c r="H46" s="55" t="n"/>
-      <c r="I46" s="55" t="n"/>
+      <c r="H46" s="27" t="n"/>
+      <c r="I46" s="27" t="n"/>
       <c r="J46" s="20" t="n"/>
-      <c r="K46" s="55" t="n"/>
-      <c r="L46" s="55" t="n"/>
+      <c r="K46" s="27" t="n"/>
+      <c r="L46" s="27" t="n"/>
       <c r="M46" s="20" t="n"/>
-      <c r="N46" s="55" t="n"/>
-      <c r="O46" s="54" t="n"/>
+      <c r="N46" s="27" t="n"/>
+      <c r="O46" s="26" t="n"/>
     </row>
     <row r="47" ht="8.1" customHeight="1" s="18">
       <c r="B47" s="65" t="inlineStr">
@@ -1427,16 +1427,16 @@
         </is>
       </c>
       <c r="C47" s="60" t="n"/>
-      <c r="E47" s="55" t="n"/>
-      <c r="F47" s="55" t="n"/>
-      <c r="H47" s="55" t="n"/>
-      <c r="I47" s="55" t="n"/>
+      <c r="E47" s="27" t="n"/>
+      <c r="F47" s="27" t="n"/>
+      <c r="H47" s="27" t="n"/>
+      <c r="I47" s="27" t="n"/>
       <c r="J47" s="20" t="n"/>
-      <c r="K47" s="55" t="n"/>
-      <c r="L47" s="55" t="n"/>
+      <c r="K47" s="27" t="n"/>
+      <c r="L47" s="27" t="n"/>
       <c r="M47" s="20" t="n"/>
-      <c r="N47" s="55" t="n"/>
-      <c r="O47" s="54" t="n"/>
+      <c r="N47" s="27" t="n"/>
+      <c r="O47" s="26" t="n"/>
     </row>
     <row r="48" ht="8.1" customHeight="1" s="18">
       <c r="B48" s="67" t="inlineStr">
@@ -1445,47 +1445,47 @@
         </is>
       </c>
       <c r="C48" s="62" t="n"/>
-      <c r="E48" s="55" t="n"/>
-      <c r="F48" s="55" t="n"/>
-      <c r="H48" s="55" t="n"/>
-      <c r="I48" s="55" t="n"/>
+      <c r="E48" s="27" t="n"/>
+      <c r="F48" s="27" t="n"/>
+      <c r="H48" s="27" t="n"/>
+      <c r="I48" s="27" t="n"/>
       <c r="J48" s="20" t="n"/>
-      <c r="K48" s="55" t="n"/>
-      <c r="L48" s="55" t="n"/>
+      <c r="K48" s="27" t="n"/>
+      <c r="L48" s="27" t="n"/>
       <c r="M48" s="20" t="n"/>
-      <c r="N48" s="55" t="n"/>
-      <c r="O48" s="54" t="n"/>
+      <c r="N48" s="27" t="n"/>
+      <c r="O48" s="26" t="n"/>
     </row>
     <row r="49" ht="8.1" customHeight="1" s="18">
-      <c r="B49" s="55" t="n"/>
-      <c r="C49" s="55" t="n"/>
-      <c r="E49" s="55" t="n"/>
-      <c r="F49" s="55" t="n"/>
-      <c r="H49" s="55" t="n"/>
-      <c r="I49" s="55" t="n"/>
+      <c r="B49" s="27" t="n"/>
+      <c r="C49" s="27" t="n"/>
+      <c r="E49" s="27" t="n"/>
+      <c r="F49" s="27" t="n"/>
+      <c r="H49" s="27" t="n"/>
+      <c r="I49" s="27" t="n"/>
       <c r="J49" s="22" t="n"/>
       <c r="K49" s="65" t="n"/>
       <c r="L49" s="60" t="n"/>
-      <c r="N49" s="55" t="n"/>
-      <c r="O49" s="54" t="n"/>
-      <c r="P49" s="44" t="inlineStr">
+      <c r="N49" s="27" t="n"/>
+      <c r="O49" s="26" t="n"/>
+      <c r="P49" s="43" t="inlineStr">
         <is>
           <t>To Final</t>
         </is>
       </c>
     </row>
     <row r="50" ht="8.1" customHeight="1" s="18">
-      <c r="B50" s="55" t="n"/>
-      <c r="C50" s="55" t="n"/>
-      <c r="E50" s="55" t="n"/>
-      <c r="F50" s="55" t="n"/>
-      <c r="H50" s="55" t="n"/>
-      <c r="I50" s="55" t="n"/>
+      <c r="B50" s="27" t="n"/>
+      <c r="C50" s="27" t="n"/>
+      <c r="E50" s="27" t="n"/>
+      <c r="F50" s="27" t="n"/>
+      <c r="H50" s="27" t="n"/>
+      <c r="I50" s="27" t="n"/>
       <c r="J50" s="20" t="n"/>
       <c r="K50" s="67" t="n"/>
       <c r="L50" s="62" t="n"/>
-      <c r="N50" s="55" t="n"/>
-      <c r="O50" s="54" t="n"/>
+      <c r="N50" s="27" t="n"/>
+      <c r="O50" s="26" t="n"/>
       <c r="P50" s="20" t="n"/>
     </row>
     <row r="51" ht="8.1" customHeight="1" s="18">
@@ -1495,15 +1495,15 @@
         </is>
       </c>
       <c r="C51" s="60" t="n"/>
-      <c r="E51" s="55" t="n"/>
-      <c r="F51" s="55" t="n"/>
-      <c r="H51" s="55" t="n"/>
-      <c r="I51" s="55" t="n"/>
+      <c r="E51" s="27" t="n"/>
+      <c r="F51" s="27" t="n"/>
+      <c r="H51" s="27" t="n"/>
+      <c r="I51" s="27" t="n"/>
       <c r="J51" s="20" t="n"/>
-      <c r="K51" s="55" t="n"/>
-      <c r="L51" s="55" t="n"/>
-      <c r="N51" s="55" t="n"/>
-      <c r="O51" s="54" t="n"/>
+      <c r="K51" s="27" t="n"/>
+      <c r="L51" s="27" t="n"/>
+      <c r="N51" s="27" t="n"/>
+      <c r="O51" s="26" t="n"/>
     </row>
     <row r="52" ht="8.1" customHeight="1" s="18">
       <c r="B52" s="61" t="inlineStr">
@@ -1512,19 +1512,19 @@
         </is>
       </c>
       <c r="C52" s="62" t="n"/>
-      <c r="E52" s="55" t="n"/>
-      <c r="F52" s="55" t="n"/>
-      <c r="H52" s="55" t="n"/>
-      <c r="I52" s="55" t="n"/>
+      <c r="E52" s="27" t="n"/>
+      <c r="F52" s="27" t="n"/>
+      <c r="H52" s="27" t="n"/>
+      <c r="I52" s="27" t="n"/>
       <c r="J52" s="20" t="n"/>
-      <c r="K52" s="55" t="n"/>
-      <c r="L52" s="55" t="n"/>
-      <c r="N52" s="55" t="n"/>
-      <c r="O52" s="54" t="n"/>
+      <c r="K52" s="27" t="n"/>
+      <c r="L52" s="27" t="n"/>
+      <c r="N52" s="27" t="n"/>
+      <c r="O52" s="26" t="n"/>
     </row>
     <row r="53" ht="8.1" customHeight="1" s="18">
-      <c r="B53" s="55" t="n"/>
-      <c r="C53" s="55" t="n"/>
+      <c r="B53" s="27" t="n"/>
+      <c r="C53" s="27" t="n"/>
       <c r="D53" s="22" t="n"/>
       <c r="E53" s="59" t="inlineStr">
         <is>
@@ -1532,17 +1532,17 @@
         </is>
       </c>
       <c r="F53" s="60" t="n"/>
-      <c r="H53" s="55" t="n"/>
-      <c r="I53" s="55" t="n"/>
+      <c r="H53" s="27" t="n"/>
+      <c r="I53" s="27" t="n"/>
       <c r="J53" s="20" t="n"/>
-      <c r="K53" s="55" t="n"/>
-      <c r="L53" s="55" t="n"/>
-      <c r="N53" s="55" t="n"/>
-      <c r="O53" s="54" t="n"/>
+      <c r="K53" s="27" t="n"/>
+      <c r="L53" s="27" t="n"/>
+      <c r="N53" s="27" t="n"/>
+      <c r="O53" s="26" t="n"/>
     </row>
     <row r="54" ht="8.1" customHeight="1" s="18">
-      <c r="B54" s="55" t="n"/>
-      <c r="C54" s="55" t="n"/>
+      <c r="B54" s="27" t="n"/>
+      <c r="C54" s="27" t="n"/>
       <c r="D54" s="19" t="n"/>
       <c r="E54" s="61" t="inlineStr">
         <is>
@@ -1550,13 +1550,13 @@
         </is>
       </c>
       <c r="F54" s="62" t="n"/>
-      <c r="H54" s="55" t="n"/>
-      <c r="I54" s="55" t="n"/>
+      <c r="H54" s="27" t="n"/>
+      <c r="I54" s="27" t="n"/>
       <c r="J54" s="20" t="n"/>
-      <c r="K54" s="55" t="n"/>
-      <c r="L54" s="55" t="n"/>
-      <c r="N54" s="55" t="n"/>
-      <c r="O54" s="54" t="n"/>
+      <c r="K54" s="27" t="n"/>
+      <c r="L54" s="27" t="n"/>
+      <c r="N54" s="27" t="n"/>
+      <c r="O54" s="26" t="n"/>
     </row>
     <row r="55" ht="8.1" customHeight="1" s="18">
       <c r="B55" s="65" t="inlineStr">
@@ -1565,56 +1565,56 @@
         </is>
       </c>
       <c r="C55" s="60" t="n"/>
-      <c r="E55" s="55" t="n"/>
-      <c r="F55" s="55" t="n"/>
+      <c r="E55" s="27" t="n"/>
+      <c r="F55" s="27" t="n"/>
       <c r="G55" s="20" t="n"/>
-      <c r="H55" s="55" t="n"/>
-      <c r="I55" s="55" t="n"/>
+      <c r="H55" s="27" t="n"/>
+      <c r="I55" s="27" t="n"/>
       <c r="J55" s="20" t="n"/>
-      <c r="K55" s="55" t="n"/>
-      <c r="L55" s="55" t="n"/>
-      <c r="N55" s="55" t="n"/>
-      <c r="O55" s="54" t="n"/>
+      <c r="K55" s="27" t="n"/>
+      <c r="L55" s="27" t="n"/>
+      <c r="N55" s="27" t="n"/>
+      <c r="O55" s="26" t="n"/>
     </row>
     <row r="56" ht="8.1" customHeight="1" s="18">
       <c r="B56" s="67" t="inlineStr"/>
       <c r="C56" s="62" t="n"/>
-      <c r="E56" s="55" t="n"/>
-      <c r="F56" s="55" t="n"/>
+      <c r="E56" s="27" t="n"/>
+      <c r="F56" s="27" t="n"/>
       <c r="G56" s="20" t="n"/>
-      <c r="H56" s="55" t="n"/>
-      <c r="I56" s="55" t="n"/>
+      <c r="H56" s="27" t="n"/>
+      <c r="I56" s="27" t="n"/>
       <c r="J56" s="20" t="n"/>
-      <c r="K56" s="55" t="n"/>
-      <c r="L56" s="55" t="n"/>
-      <c r="N56" s="55" t="n"/>
-      <c r="O56" s="54" t="n"/>
+      <c r="K56" s="27" t="n"/>
+      <c r="L56" s="27" t="n"/>
+      <c r="N56" s="27" t="n"/>
+      <c r="O56" s="26" t="n"/>
     </row>
     <row r="57" ht="8.1" customHeight="1" s="18">
-      <c r="B57" s="55" t="n"/>
-      <c r="C57" s="55" t="n"/>
-      <c r="E57" s="55" t="n"/>
-      <c r="F57" s="55" t="n"/>
+      <c r="B57" s="27" t="n"/>
+      <c r="C57" s="27" t="n"/>
+      <c r="E57" s="27" t="n"/>
+      <c r="F57" s="27" t="n"/>
       <c r="G57" s="22" t="n"/>
       <c r="H57" s="65" t="n"/>
       <c r="I57" s="60" t="n"/>
-      <c r="K57" s="55" t="n"/>
-      <c r="L57" s="55" t="n"/>
-      <c r="N57" s="55" t="n"/>
-      <c r="O57" s="54" t="n"/>
+      <c r="K57" s="27" t="n"/>
+      <c r="L57" s="27" t="n"/>
+      <c r="N57" s="27" t="n"/>
+      <c r="O57" s="26" t="n"/>
     </row>
     <row r="58" ht="8.1" customHeight="1" s="18">
-      <c r="B58" s="55" t="n"/>
-      <c r="C58" s="55" t="n"/>
-      <c r="E58" s="55" t="n"/>
-      <c r="F58" s="55" t="n"/>
+      <c r="B58" s="27" t="n"/>
+      <c r="C58" s="27" t="n"/>
+      <c r="E58" s="27" t="n"/>
+      <c r="F58" s="27" t="n"/>
       <c r="G58" s="20" t="n"/>
       <c r="H58" s="67" t="n"/>
       <c r="I58" s="62" t="n"/>
-      <c r="K58" s="55" t="n"/>
-      <c r="L58" s="55" t="n"/>
-      <c r="N58" s="55" t="n"/>
-      <c r="O58" s="54" t="n"/>
+      <c r="K58" s="27" t="n"/>
+      <c r="L58" s="27" t="n"/>
+      <c r="N58" s="27" t="n"/>
+      <c r="O58" s="26" t="n"/>
     </row>
     <row r="59" ht="8.1" customHeight="1" s="18">
       <c r="B59" s="59" t="inlineStr">
@@ -1623,15 +1623,15 @@
         </is>
       </c>
       <c r="C59" s="60" t="n"/>
-      <c r="E59" s="55" t="n"/>
-      <c r="F59" s="55" t="n"/>
+      <c r="E59" s="27" t="n"/>
+      <c r="F59" s="27" t="n"/>
       <c r="G59" s="20" t="n"/>
-      <c r="H59" s="55" t="n"/>
-      <c r="I59" s="55" t="n"/>
-      <c r="K59" s="55" t="n"/>
-      <c r="L59" s="55" t="n"/>
-      <c r="N59" s="55" t="n"/>
-      <c r="O59" s="54" t="n"/>
+      <c r="H59" s="27" t="n"/>
+      <c r="I59" s="27" t="n"/>
+      <c r="K59" s="27" t="n"/>
+      <c r="L59" s="27" t="n"/>
+      <c r="N59" s="27" t="n"/>
+      <c r="O59" s="26" t="n"/>
     </row>
     <row r="60" ht="8.1" customHeight="1" s="18">
       <c r="B60" s="61" t="inlineStr">
@@ -1640,48 +1640,48 @@
         </is>
       </c>
       <c r="C60" s="62" t="n"/>
-      <c r="E60" s="55" t="n"/>
-      <c r="F60" s="55" t="n"/>
+      <c r="E60" s="27" t="n"/>
+      <c r="F60" s="27" t="n"/>
       <c r="G60" s="20" t="n"/>
-      <c r="H60" s="55" t="n"/>
-      <c r="I60" s="55" t="n"/>
-      <c r="K60" s="55" t="n"/>
-      <c r="L60" s="55" t="n"/>
-      <c r="N60" s="55" t="n"/>
-      <c r="O60" s="54" t="n"/>
-      <c r="P60" s="51" t="inlineStr">
+      <c r="H60" s="27" t="n"/>
+      <c r="I60" s="27" t="n"/>
+      <c r="K60" s="27" t="n"/>
+      <c r="L60" s="27" t="n"/>
+      <c r="N60" s="27" t="n"/>
+      <c r="O60" s="26" t="n"/>
+      <c r="P60" s="37" t="inlineStr">
         <is>
           <t>Winner</t>
         </is>
       </c>
     </row>
     <row r="61" ht="8.1" customHeight="1" s="18">
-      <c r="B61" s="55" t="n"/>
-      <c r="C61" s="55" t="n"/>
+      <c r="B61" s="27" t="n"/>
+      <c r="C61" s="27" t="n"/>
       <c r="D61" s="22" t="n"/>
       <c r="E61" s="65" t="inlineStr"/>
       <c r="F61" s="60" t="n"/>
-      <c r="H61" s="55" t="n"/>
-      <c r="I61" s="55" t="n"/>
-      <c r="K61" s="55" t="n"/>
-      <c r="L61" s="55" t="n"/>
-      <c r="N61" s="55" t="n"/>
-      <c r="O61" s="54" t="n"/>
+      <c r="H61" s="27" t="n"/>
+      <c r="I61" s="27" t="n"/>
+      <c r="K61" s="27" t="n"/>
+      <c r="L61" s="27" t="n"/>
+      <c r="N61" s="27" t="n"/>
+      <c r="O61" s="26" t="n"/>
       <c r="P61" s="58" t="n"/>
       <c r="Q61" s="58" t="n"/>
     </row>
     <row r="62" ht="8.1" customHeight="1" s="18">
-      <c r="B62" s="55" t="n"/>
-      <c r="C62" s="55" t="n"/>
+      <c r="B62" s="27" t="n"/>
+      <c r="C62" s="27" t="n"/>
       <c r="D62" s="19" t="n"/>
       <c r="E62" s="67" t="inlineStr"/>
       <c r="F62" s="62" t="n"/>
-      <c r="H62" s="55" t="n"/>
-      <c r="I62" s="55" t="n"/>
-      <c r="K62" s="55" t="n"/>
-      <c r="L62" s="55" t="n"/>
-      <c r="N62" s="55" t="n"/>
-      <c r="O62" s="54" t="n"/>
+      <c r="H62" s="27" t="n"/>
+      <c r="I62" s="27" t="n"/>
+      <c r="K62" s="27" t="n"/>
+      <c r="L62" s="27" t="n"/>
+      <c r="N62" s="27" t="n"/>
+      <c r="O62" s="26" t="n"/>
       <c r="P62" s="69" t="n"/>
       <c r="Q62" s="60" t="n"/>
     </row>
@@ -1692,14 +1692,14 @@
         </is>
       </c>
       <c r="C63" s="60" t="n"/>
-      <c r="E63" s="55" t="n"/>
-      <c r="F63" s="55" t="n"/>
-      <c r="H63" s="55" t="n"/>
-      <c r="I63" s="55" t="n"/>
-      <c r="K63" s="55" t="n"/>
-      <c r="L63" s="55" t="n"/>
-      <c r="N63" s="55" t="n"/>
-      <c r="O63" s="54" t="n"/>
+      <c r="E63" s="27" t="n"/>
+      <c r="F63" s="27" t="n"/>
+      <c r="H63" s="27" t="n"/>
+      <c r="I63" s="27" t="n"/>
+      <c r="K63" s="27" t="n"/>
+      <c r="L63" s="27" t="n"/>
+      <c r="N63" s="27" t="n"/>
+      <c r="O63" s="26" t="n"/>
       <c r="P63" s="70" t="n"/>
       <c r="Q63" s="62" t="n"/>
     </row>
@@ -1710,38 +1710,38 @@
         </is>
       </c>
       <c r="C64" s="62" t="n"/>
-      <c r="E64" s="55" t="n"/>
-      <c r="F64" s="55" t="n"/>
-      <c r="H64" s="55" t="n"/>
-      <c r="I64" s="55" t="n"/>
-      <c r="K64" s="55" t="n"/>
-      <c r="L64" s="55" t="n"/>
-      <c r="N64" s="55" t="n"/>
-      <c r="O64" s="54" t="n"/>
+      <c r="E64" s="27" t="n"/>
+      <c r="F64" s="27" t="n"/>
+      <c r="H64" s="27" t="n"/>
+      <c r="I64" s="27" t="n"/>
+      <c r="K64" s="27" t="n"/>
+      <c r="L64" s="27" t="n"/>
+      <c r="N64" s="27" t="n"/>
+      <c r="O64" s="26" t="n"/>
     </row>
     <row r="65" ht="8.1" customHeight="1" s="18">
-      <c r="B65" s="55" t="n"/>
-      <c r="C65" s="55" t="n"/>
-      <c r="E65" s="55" t="n"/>
-      <c r="F65" s="55" t="n"/>
-      <c r="H65" s="55" t="n"/>
-      <c r="I65" s="55" t="n"/>
-      <c r="K65" s="55" t="n"/>
-      <c r="L65" s="55" t="n"/>
-      <c r="N65" s="55" t="n"/>
-      <c r="O65" s="54" t="n"/>
+      <c r="B65" s="27" t="n"/>
+      <c r="C65" s="27" t="n"/>
+      <c r="E65" s="27" t="n"/>
+      <c r="F65" s="27" t="n"/>
+      <c r="H65" s="27" t="n"/>
+      <c r="I65" s="27" t="n"/>
+      <c r="K65" s="27" t="n"/>
+      <c r="L65" s="27" t="n"/>
+      <c r="N65" s="27" t="n"/>
+      <c r="O65" s="26" t="n"/>
     </row>
     <row r="66" ht="8.1" customHeight="1" s="18">
-      <c r="B66" s="55" t="n"/>
-      <c r="C66" s="55" t="n"/>
-      <c r="E66" s="55" t="n"/>
-      <c r="F66" s="55" t="n"/>
-      <c r="H66" s="55" t="n"/>
-      <c r="I66" s="55" t="n"/>
-      <c r="K66" s="55" t="n"/>
-      <c r="L66" s="55" t="n"/>
-      <c r="N66" s="55" t="n"/>
-      <c r="O66" s="54" t="n"/>
+      <c r="B66" s="27" t="n"/>
+      <c r="C66" s="27" t="n"/>
+      <c r="E66" s="27" t="n"/>
+      <c r="F66" s="27" t="n"/>
+      <c r="H66" s="27" t="n"/>
+      <c r="I66" s="27" t="n"/>
+      <c r="K66" s="27" t="n"/>
+      <c r="L66" s="27" t="n"/>
+      <c r="N66" s="27" t="n"/>
+      <c r="O66" s="26" t="n"/>
     </row>
     <row r="67" ht="8.1" customHeight="1" s="18">
       <c r="B67" s="59" t="inlineStr">
@@ -1750,14 +1750,14 @@
         </is>
       </c>
       <c r="C67" s="60" t="n"/>
-      <c r="E67" s="55" t="n"/>
-      <c r="F67" s="55" t="n"/>
-      <c r="H67" s="55" t="n"/>
-      <c r="I67" s="55" t="n"/>
-      <c r="K67" s="55" t="n"/>
-      <c r="L67" s="55" t="n"/>
-      <c r="N67" s="55" t="n"/>
-      <c r="O67" s="54" t="n"/>
+      <c r="E67" s="27" t="n"/>
+      <c r="F67" s="27" t="n"/>
+      <c r="H67" s="27" t="n"/>
+      <c r="I67" s="27" t="n"/>
+      <c r="K67" s="27" t="n"/>
+      <c r="L67" s="27" t="n"/>
+      <c r="N67" s="27" t="n"/>
+      <c r="O67" s="26" t="n"/>
     </row>
     <row r="68" ht="8.1" customHeight="1" s="18">
       <c r="B68" s="61" t="inlineStr">
@@ -1766,18 +1766,18 @@
         </is>
       </c>
       <c r="C68" s="62" t="n"/>
-      <c r="E68" s="55" t="n"/>
-      <c r="F68" s="55" t="n"/>
-      <c r="H68" s="55" t="n"/>
-      <c r="I68" s="55" t="n"/>
-      <c r="K68" s="55" t="n"/>
-      <c r="L68" s="55" t="n"/>
-      <c r="N68" s="55" t="n"/>
-      <c r="O68" s="54" t="n"/>
+      <c r="E68" s="27" t="n"/>
+      <c r="F68" s="27" t="n"/>
+      <c r="H68" s="27" t="n"/>
+      <c r="I68" s="27" t="n"/>
+      <c r="K68" s="27" t="n"/>
+      <c r="L68" s="27" t="n"/>
+      <c r="N68" s="27" t="n"/>
+      <c r="O68" s="26" t="n"/>
     </row>
     <row r="69" ht="8.1" customHeight="1" s="18">
-      <c r="B69" s="55" t="n"/>
-      <c r="C69" s="55" t="n"/>
+      <c r="B69" s="27" t="n"/>
+      <c r="C69" s="27" t="n"/>
       <c r="D69" s="22" t="n"/>
       <c r="E69" s="59" t="inlineStr">
         <is>
@@ -1785,16 +1785,16 @@
         </is>
       </c>
       <c r="F69" s="60" t="n"/>
-      <c r="H69" s="55" t="n"/>
-      <c r="I69" s="55" t="n"/>
-      <c r="K69" s="55" t="n"/>
-      <c r="L69" s="55" t="n"/>
-      <c r="N69" s="55" t="n"/>
-      <c r="O69" s="54" t="n"/>
+      <c r="H69" s="27" t="n"/>
+      <c r="I69" s="27" t="n"/>
+      <c r="K69" s="27" t="n"/>
+      <c r="L69" s="27" t="n"/>
+      <c r="N69" s="27" t="n"/>
+      <c r="O69" s="26" t="n"/>
     </row>
     <row r="70" ht="8.1" customHeight="1" s="18">
-      <c r="B70" s="55" t="n"/>
-      <c r="C70" s="55" t="n"/>
+      <c r="B70" s="27" t="n"/>
+      <c r="C70" s="27" t="n"/>
       <c r="D70" s="19" t="n"/>
       <c r="E70" s="61" t="inlineStr">
         <is>
@@ -1802,12 +1802,12 @@
         </is>
       </c>
       <c r="F70" s="62" t="n"/>
-      <c r="H70" s="55" t="n"/>
-      <c r="I70" s="55" t="n"/>
-      <c r="K70" s="55" t="n"/>
-      <c r="L70" s="55" t="n"/>
-      <c r="N70" s="55" t="n"/>
-      <c r="O70" s="54" t="n"/>
+      <c r="H70" s="27" t="n"/>
+      <c r="I70" s="27" t="n"/>
+      <c r="K70" s="27" t="n"/>
+      <c r="L70" s="27" t="n"/>
+      <c r="N70" s="27" t="n"/>
+      <c r="O70" s="26" t="n"/>
     </row>
     <row r="71" ht="8.1" customHeight="1" s="18">
       <c r="B71" s="65" t="inlineStr">
@@ -1816,54 +1816,54 @@
         </is>
       </c>
       <c r="C71" s="60" t="n"/>
-      <c r="E71" s="55" t="n"/>
-      <c r="F71" s="55" t="n"/>
+      <c r="E71" s="27" t="n"/>
+      <c r="F71" s="27" t="n"/>
       <c r="G71" s="20" t="n"/>
-      <c r="H71" s="55" t="n"/>
-      <c r="I71" s="55" t="n"/>
-      <c r="K71" s="55" t="n"/>
-      <c r="L71" s="55" t="n"/>
-      <c r="N71" s="55" t="n"/>
-      <c r="O71" s="54" t="n"/>
+      <c r="H71" s="27" t="n"/>
+      <c r="I71" s="27" t="n"/>
+      <c r="K71" s="27" t="n"/>
+      <c r="L71" s="27" t="n"/>
+      <c r="N71" s="27" t="n"/>
+      <c r="O71" s="26" t="n"/>
     </row>
     <row r="72" ht="8.1" customHeight="1" s="18">
       <c r="B72" s="67" t="inlineStr"/>
       <c r="C72" s="62" t="n"/>
-      <c r="E72" s="55" t="n"/>
-      <c r="F72" s="55" t="n"/>
+      <c r="E72" s="27" t="n"/>
+      <c r="F72" s="27" t="n"/>
       <c r="G72" s="20" t="n"/>
-      <c r="H72" s="55" t="n"/>
-      <c r="I72" s="55" t="n"/>
-      <c r="K72" s="55" t="n"/>
-      <c r="L72" s="55" t="n"/>
-      <c r="N72" s="55" t="n"/>
-      <c r="O72" s="54" t="n"/>
+      <c r="H72" s="27" t="n"/>
+      <c r="I72" s="27" t="n"/>
+      <c r="K72" s="27" t="n"/>
+      <c r="L72" s="27" t="n"/>
+      <c r="N72" s="27" t="n"/>
+      <c r="O72" s="26" t="n"/>
     </row>
     <row r="73" ht="8.1" customHeight="1" s="18">
-      <c r="B73" s="55" t="n"/>
-      <c r="C73" s="55" t="n"/>
-      <c r="E73" s="55" t="n"/>
-      <c r="F73" s="55" t="n"/>
+      <c r="B73" s="27" t="n"/>
+      <c r="C73" s="27" t="n"/>
+      <c r="E73" s="27" t="n"/>
+      <c r="F73" s="27" t="n"/>
       <c r="G73" s="22" t="n"/>
       <c r="H73" s="59" t="n"/>
       <c r="I73" s="60" t="n"/>
-      <c r="K73" s="55" t="n"/>
-      <c r="L73" s="55" t="n"/>
-      <c r="N73" s="55" t="n"/>
-      <c r="O73" s="54" t="n"/>
+      <c r="K73" s="27" t="n"/>
+      <c r="L73" s="27" t="n"/>
+      <c r="N73" s="27" t="n"/>
+      <c r="O73" s="26" t="n"/>
     </row>
     <row r="74" ht="8.1" customHeight="1" s="18">
-      <c r="B74" s="55" t="n"/>
-      <c r="C74" s="55" t="n"/>
-      <c r="E74" s="55" t="n"/>
-      <c r="F74" s="55" t="n"/>
+      <c r="B74" s="27" t="n"/>
+      <c r="C74" s="27" t="n"/>
+      <c r="E74" s="27" t="n"/>
+      <c r="F74" s="27" t="n"/>
       <c r="G74" s="20" t="n"/>
       <c r="H74" s="61" t="n"/>
       <c r="I74" s="62" t="n"/>
-      <c r="K74" s="55" t="n"/>
-      <c r="L74" s="55" t="n"/>
-      <c r="N74" s="55" t="n"/>
-      <c r="O74" s="54" t="n"/>
+      <c r="K74" s="27" t="n"/>
+      <c r="L74" s="27" t="n"/>
+      <c r="N74" s="27" t="n"/>
+      <c r="O74" s="26" t="n"/>
     </row>
     <row r="75" ht="8.1" customHeight="1" s="18">
       <c r="B75" s="59" t="inlineStr">
@@ -1872,34 +1872,34 @@
         </is>
       </c>
       <c r="C75" s="60" t="n"/>
-      <c r="E75" s="55" t="n"/>
-      <c r="F75" s="55" t="n"/>
+      <c r="E75" s="27" t="n"/>
+      <c r="F75" s="27" t="n"/>
       <c r="G75" s="20" t="n"/>
-      <c r="H75" s="55" t="n"/>
-      <c r="I75" s="55" t="n"/>
+      <c r="H75" s="27" t="n"/>
+      <c r="I75" s="27" t="n"/>
       <c r="J75" s="20" t="n"/>
-      <c r="K75" s="55" t="n"/>
-      <c r="L75" s="55" t="n"/>
-      <c r="N75" s="55" t="n"/>
-      <c r="O75" s="54" t="n"/>
+      <c r="K75" s="27" t="n"/>
+      <c r="L75" s="27" t="n"/>
+      <c r="N75" s="27" t="n"/>
+      <c r="O75" s="26" t="n"/>
     </row>
     <row r="76" ht="8.1" customHeight="1" s="18">
       <c r="B76" s="61" t="inlineStr"/>
       <c r="C76" s="62" t="n"/>
-      <c r="E76" s="55" t="n"/>
-      <c r="F76" s="55" t="n"/>
+      <c r="E76" s="27" t="n"/>
+      <c r="F76" s="27" t="n"/>
       <c r="G76" s="20" t="n"/>
-      <c r="H76" s="55" t="n"/>
-      <c r="I76" s="55" t="n"/>
+      <c r="H76" s="27" t="n"/>
+      <c r="I76" s="27" t="n"/>
       <c r="J76" s="20" t="n"/>
-      <c r="K76" s="55" t="n"/>
-      <c r="L76" s="55" t="n"/>
-      <c r="N76" s="55" t="n"/>
-      <c r="O76" s="54" t="n"/>
+      <c r="K76" s="27" t="n"/>
+      <c r="L76" s="27" t="n"/>
+      <c r="N76" s="27" t="n"/>
+      <c r="O76" s="26" t="n"/>
     </row>
     <row r="77" ht="8.1" customHeight="1" s="18">
-      <c r="B77" s="55" t="n"/>
-      <c r="C77" s="55" t="n"/>
+      <c r="B77" s="27" t="n"/>
+      <c r="C77" s="27" t="n"/>
       <c r="D77" s="22" t="n"/>
       <c r="E77" s="65" t="inlineStr">
         <is>
@@ -1907,17 +1907,17 @@
         </is>
       </c>
       <c r="F77" s="60" t="n"/>
-      <c r="H77" s="55" t="n"/>
-      <c r="I77" s="55" t="n"/>
+      <c r="H77" s="27" t="n"/>
+      <c r="I77" s="27" t="n"/>
       <c r="J77" s="20" t="n"/>
-      <c r="K77" s="55" t="n"/>
-      <c r="L77" s="55" t="n"/>
-      <c r="N77" s="55" t="n"/>
-      <c r="O77" s="54" t="n"/>
+      <c r="K77" s="27" t="n"/>
+      <c r="L77" s="27" t="n"/>
+      <c r="N77" s="27" t="n"/>
+      <c r="O77" s="26" t="n"/>
     </row>
     <row r="78" ht="8.1" customHeight="1" s="18">
-      <c r="B78" s="55" t="n"/>
-      <c r="C78" s="55" t="n"/>
+      <c r="B78" s="27" t="n"/>
+      <c r="C78" s="27" t="n"/>
       <c r="D78" s="19" t="n"/>
       <c r="E78" s="67" t="inlineStr">
         <is>
@@ -1925,13 +1925,13 @@
         </is>
       </c>
       <c r="F78" s="62" t="n"/>
-      <c r="H78" s="55" t="n"/>
-      <c r="I78" s="55" t="n"/>
+      <c r="H78" s="27" t="n"/>
+      <c r="I78" s="27" t="n"/>
       <c r="J78" s="20" t="n"/>
-      <c r="K78" s="55" t="n"/>
-      <c r="L78" s="55" t="n"/>
-      <c r="N78" s="55" t="n"/>
-      <c r="O78" s="54" t="n"/>
+      <c r="K78" s="27" t="n"/>
+      <c r="L78" s="27" t="n"/>
+      <c r="N78" s="27" t="n"/>
+      <c r="O78" s="26" t="n"/>
     </row>
     <row r="79" ht="8.1" customHeight="1" s="18">
       <c r="B79" s="65" t="inlineStr">
@@ -1940,15 +1940,15 @@
         </is>
       </c>
       <c r="C79" s="60" t="n"/>
-      <c r="E79" s="55" t="n"/>
-      <c r="F79" s="55" t="n"/>
-      <c r="H79" s="55" t="n"/>
-      <c r="I79" s="55" t="n"/>
+      <c r="E79" s="27" t="n"/>
+      <c r="F79" s="27" t="n"/>
+      <c r="H79" s="27" t="n"/>
+      <c r="I79" s="27" t="n"/>
       <c r="J79" s="20" t="n"/>
-      <c r="K79" s="55" t="n"/>
-      <c r="L79" s="55" t="n"/>
-      <c r="N79" s="55" t="n"/>
-      <c r="O79" s="54" t="n"/>
+      <c r="K79" s="27" t="n"/>
+      <c r="L79" s="27" t="n"/>
+      <c r="N79" s="27" t="n"/>
+      <c r="O79" s="26" t="n"/>
     </row>
     <row r="80" ht="8.1" customHeight="1" s="18">
       <c r="B80" s="67" t="inlineStr">
@@ -1957,46 +1957,46 @@
         </is>
       </c>
       <c r="C80" s="62" t="n"/>
-      <c r="E80" s="55" t="n"/>
-      <c r="F80" s="55" t="n"/>
-      <c r="H80" s="55" t="n"/>
-      <c r="I80" s="55" t="n"/>
+      <c r="E80" s="27" t="n"/>
+      <c r="F80" s="27" t="n"/>
+      <c r="H80" s="27" t="n"/>
+      <c r="I80" s="27" t="n"/>
       <c r="J80" s="20" t="n"/>
-      <c r="K80" s="55" t="n"/>
-      <c r="L80" s="55" t="n"/>
-      <c r="N80" s="55" t="n"/>
-      <c r="O80" s="54" t="n"/>
+      <c r="K80" s="27" t="n"/>
+      <c r="L80" s="27" t="n"/>
+      <c r="N80" s="27" t="n"/>
+      <c r="O80" s="26" t="n"/>
     </row>
     <row r="81" ht="8.1" customHeight="1" s="18">
-      <c r="B81" s="55" t="n"/>
-      <c r="C81" s="55" t="n"/>
-      <c r="E81" s="55" t="n"/>
-      <c r="F81" s="55" t="n"/>
-      <c r="H81" s="55" t="n"/>
-      <c r="I81" s="55" t="n"/>
+      <c r="B81" s="27" t="n"/>
+      <c r="C81" s="27" t="n"/>
+      <c r="E81" s="27" t="n"/>
+      <c r="F81" s="27" t="n"/>
+      <c r="H81" s="27" t="n"/>
+      <c r="I81" s="27" t="n"/>
       <c r="J81" s="22" t="n"/>
       <c r="K81" s="59" t="n"/>
       <c r="L81" s="60" t="n"/>
-      <c r="N81" s="55" t="n"/>
-      <c r="O81" s="54" t="n"/>
-      <c r="P81" s="44" t="inlineStr">
+      <c r="N81" s="27" t="n"/>
+      <c r="O81" s="26" t="n"/>
+      <c r="P81" s="43" t="inlineStr">
         <is>
           <t>To Final</t>
         </is>
       </c>
     </row>
     <row r="82" ht="8.1" customHeight="1" s="18">
-      <c r="B82" s="55" t="n"/>
-      <c r="C82" s="55" t="n"/>
-      <c r="E82" s="55" t="n"/>
-      <c r="F82" s="55" t="n"/>
-      <c r="H82" s="55" t="n"/>
-      <c r="I82" s="55" t="n"/>
+      <c r="B82" s="27" t="n"/>
+      <c r="C82" s="27" t="n"/>
+      <c r="E82" s="27" t="n"/>
+      <c r="F82" s="27" t="n"/>
+      <c r="H82" s="27" t="n"/>
+      <c r="I82" s="27" t="n"/>
       <c r="J82" s="20" t="n"/>
       <c r="K82" s="61" t="n"/>
       <c r="L82" s="62" t="n"/>
-      <c r="N82" s="55" t="n"/>
-      <c r="O82" s="54" t="n"/>
+      <c r="N82" s="27" t="n"/>
+      <c r="O82" s="26" t="n"/>
       <c r="P82" s="20" t="n"/>
     </row>
     <row r="83" ht="8.1" customHeight="1" s="18">
@@ -2006,16 +2006,16 @@
         </is>
       </c>
       <c r="C83" s="60" t="n"/>
-      <c r="E83" s="55" t="n"/>
-      <c r="F83" s="55" t="n"/>
-      <c r="H83" s="55" t="n"/>
-      <c r="I83" s="55" t="n"/>
+      <c r="E83" s="27" t="n"/>
+      <c r="F83" s="27" t="n"/>
+      <c r="H83" s="27" t="n"/>
+      <c r="I83" s="27" t="n"/>
       <c r="J83" s="20" t="n"/>
-      <c r="K83" s="55" t="n"/>
-      <c r="L83" s="55" t="n"/>
+      <c r="K83" s="27" t="n"/>
+      <c r="L83" s="27" t="n"/>
       <c r="M83" s="20" t="n"/>
-      <c r="N83" s="55" t="n"/>
-      <c r="O83" s="54" t="n"/>
+      <c r="N83" s="27" t="n"/>
+      <c r="O83" s="26" t="n"/>
     </row>
     <row r="84" ht="8.1" customHeight="1" s="18">
       <c r="B84" s="61" t="inlineStr">
@@ -2024,20 +2024,20 @@
         </is>
       </c>
       <c r="C84" s="62" t="n"/>
-      <c r="E84" s="55" t="n"/>
-      <c r="F84" s="55" t="n"/>
-      <c r="H84" s="55" t="n"/>
-      <c r="I84" s="55" t="n"/>
+      <c r="E84" s="27" t="n"/>
+      <c r="F84" s="27" t="n"/>
+      <c r="H84" s="27" t="n"/>
+      <c r="I84" s="27" t="n"/>
       <c r="J84" s="20" t="n"/>
-      <c r="K84" s="55" t="n"/>
-      <c r="L84" s="55" t="n"/>
+      <c r="K84" s="27" t="n"/>
+      <c r="L84" s="27" t="n"/>
       <c r="M84" s="20" t="n"/>
-      <c r="N84" s="55" t="n"/>
-      <c r="O84" s="54" t="n"/>
+      <c r="N84" s="27" t="n"/>
+      <c r="O84" s="26" t="n"/>
     </row>
     <row r="85" ht="8.1" customHeight="1" s="18">
-      <c r="B85" s="55" t="n"/>
-      <c r="C85" s="55" t="n"/>
+      <c r="B85" s="27" t="n"/>
+      <c r="C85" s="27" t="n"/>
       <c r="D85" s="22" t="n"/>
       <c r="E85" s="59" t="inlineStr">
         <is>
@@ -2045,18 +2045,18 @@
         </is>
       </c>
       <c r="F85" s="60" t="n"/>
-      <c r="H85" s="55" t="n"/>
-      <c r="I85" s="55" t="n"/>
+      <c r="H85" s="27" t="n"/>
+      <c r="I85" s="27" t="n"/>
       <c r="J85" s="20" t="n"/>
-      <c r="K85" s="55" t="n"/>
-      <c r="L85" s="55" t="n"/>
+      <c r="K85" s="27" t="n"/>
+      <c r="L85" s="27" t="n"/>
       <c r="M85" s="20" t="n"/>
-      <c r="N85" s="55" t="n"/>
-      <c r="O85" s="54" t="n"/>
+      <c r="N85" s="27" t="n"/>
+      <c r="O85" s="26" t="n"/>
     </row>
     <row r="86" ht="8.1" customHeight="1" s="18">
-      <c r="B86" s="55" t="n"/>
-      <c r="C86" s="55" t="n"/>
+      <c r="B86" s="27" t="n"/>
+      <c r="C86" s="27" t="n"/>
       <c r="D86" s="19" t="n"/>
       <c r="E86" s="61" t="inlineStr">
         <is>
@@ -2064,14 +2064,14 @@
         </is>
       </c>
       <c r="F86" s="62" t="n"/>
-      <c r="H86" s="55" t="n"/>
-      <c r="I86" s="55" t="n"/>
+      <c r="H86" s="27" t="n"/>
+      <c r="I86" s="27" t="n"/>
       <c r="J86" s="20" t="n"/>
-      <c r="K86" s="55" t="n"/>
-      <c r="L86" s="55" t="n"/>
+      <c r="K86" s="27" t="n"/>
+      <c r="L86" s="27" t="n"/>
       <c r="M86" s="20" t="n"/>
-      <c r="N86" s="55" t="n"/>
-      <c r="O86" s="54" t="n"/>
+      <c r="N86" s="27" t="n"/>
+      <c r="O86" s="26" t="n"/>
     </row>
     <row r="87" ht="8.1" customHeight="1" s="18">
       <c r="B87" s="65" t="inlineStr">
@@ -2080,60 +2080,60 @@
         </is>
       </c>
       <c r="C87" s="60" t="n"/>
-      <c r="E87" s="55" t="n"/>
-      <c r="F87" s="55" t="n"/>
+      <c r="E87" s="27" t="n"/>
+      <c r="F87" s="27" t="n"/>
       <c r="G87" s="20" t="n"/>
-      <c r="H87" s="55" t="n"/>
-      <c r="I87" s="55" t="n"/>
+      <c r="H87" s="27" t="n"/>
+      <c r="I87" s="27" t="n"/>
       <c r="J87" s="20" t="n"/>
-      <c r="K87" s="55" t="n"/>
-      <c r="L87" s="55" t="n"/>
+      <c r="K87" s="27" t="n"/>
+      <c r="L87" s="27" t="n"/>
       <c r="M87" s="20" t="n"/>
-      <c r="N87" s="55" t="n"/>
-      <c r="O87" s="54" t="n"/>
+      <c r="N87" s="27" t="n"/>
+      <c r="O87" s="26" t="n"/>
     </row>
     <row r="88" ht="8.1" customHeight="1" s="18">
       <c r="B88" s="67" t="inlineStr"/>
       <c r="C88" s="62" t="n"/>
-      <c r="E88" s="55" t="n"/>
-      <c r="F88" s="55" t="n"/>
+      <c r="E88" s="27" t="n"/>
+      <c r="F88" s="27" t="n"/>
       <c r="G88" s="20" t="n"/>
-      <c r="H88" s="55" t="n"/>
-      <c r="I88" s="55" t="n"/>
+      <c r="H88" s="27" t="n"/>
+      <c r="I88" s="27" t="n"/>
       <c r="J88" s="20" t="n"/>
-      <c r="K88" s="55" t="n"/>
-      <c r="L88" s="55" t="n"/>
+      <c r="K88" s="27" t="n"/>
+      <c r="L88" s="27" t="n"/>
       <c r="M88" s="20" t="n"/>
-      <c r="N88" s="55" t="n"/>
-      <c r="O88" s="54" t="n"/>
+      <c r="N88" s="27" t="n"/>
+      <c r="O88" s="26" t="n"/>
     </row>
     <row r="89" ht="8.1" customHeight="1" s="18">
-      <c r="B89" s="55" t="n"/>
-      <c r="C89" s="55" t="n"/>
-      <c r="E89" s="55" t="n"/>
-      <c r="F89" s="55" t="n"/>
+      <c r="B89" s="27" t="n"/>
+      <c r="C89" s="27" t="n"/>
+      <c r="E89" s="27" t="n"/>
+      <c r="F89" s="27" t="n"/>
       <c r="G89" s="22" t="n"/>
       <c r="H89" s="65" t="n"/>
       <c r="I89" s="60" t="n"/>
-      <c r="K89" s="55" t="n"/>
-      <c r="L89" s="55" t="n"/>
+      <c r="K89" s="27" t="n"/>
+      <c r="L89" s="27" t="n"/>
       <c r="M89" s="20" t="n"/>
-      <c r="N89" s="55" t="n"/>
-      <c r="O89" s="54" t="n"/>
+      <c r="N89" s="27" t="n"/>
+      <c r="O89" s="26" t="n"/>
     </row>
     <row r="90" ht="8.1" customHeight="1" s="18">
-      <c r="B90" s="55" t="n"/>
-      <c r="C90" s="55" t="n"/>
-      <c r="E90" s="55" t="n"/>
-      <c r="F90" s="55" t="n"/>
+      <c r="B90" s="27" t="n"/>
+      <c r="C90" s="27" t="n"/>
+      <c r="E90" s="27" t="n"/>
+      <c r="F90" s="27" t="n"/>
       <c r="G90" s="20" t="n"/>
       <c r="H90" s="67" t="n"/>
       <c r="I90" s="62" t="n"/>
-      <c r="K90" s="55" t="n"/>
-      <c r="L90" s="55" t="n"/>
+      <c r="K90" s="27" t="n"/>
+      <c r="L90" s="27" t="n"/>
       <c r="M90" s="20" t="n"/>
-      <c r="N90" s="55" t="n"/>
-      <c r="O90" s="54" t="n"/>
+      <c r="N90" s="27" t="n"/>
+      <c r="O90" s="26" t="n"/>
     </row>
     <row r="91" ht="8.1" customHeight="1" s="18">
       <c r="B91" s="59" t="inlineStr">
@@ -2142,34 +2142,34 @@
         </is>
       </c>
       <c r="C91" s="60" t="n"/>
-      <c r="E91" s="55" t="n"/>
-      <c r="F91" s="55" t="n"/>
+      <c r="E91" s="27" t="n"/>
+      <c r="F91" s="27" t="n"/>
       <c r="G91" s="20" t="n"/>
-      <c r="H91" s="55" t="n"/>
-      <c r="I91" s="55" t="n"/>
-      <c r="K91" s="55" t="n"/>
-      <c r="L91" s="55" t="n"/>
+      <c r="H91" s="27" t="n"/>
+      <c r="I91" s="27" t="n"/>
+      <c r="K91" s="27" t="n"/>
+      <c r="L91" s="27" t="n"/>
       <c r="M91" s="20" t="n"/>
-      <c r="N91" s="55" t="n"/>
-      <c r="O91" s="54" t="n"/>
+      <c r="N91" s="27" t="n"/>
+      <c r="O91" s="26" t="n"/>
     </row>
     <row r="92" ht="8.1" customHeight="1" s="18">
       <c r="B92" s="61" t="inlineStr"/>
       <c r="C92" s="62" t="n"/>
-      <c r="E92" s="55" t="n"/>
-      <c r="F92" s="55" t="n"/>
+      <c r="E92" s="27" t="n"/>
+      <c r="F92" s="27" t="n"/>
       <c r="G92" s="20" t="n"/>
-      <c r="H92" s="55" t="n"/>
-      <c r="I92" s="55" t="n"/>
-      <c r="K92" s="55" t="n"/>
-      <c r="L92" s="55" t="n"/>
+      <c r="H92" s="27" t="n"/>
+      <c r="I92" s="27" t="n"/>
+      <c r="K92" s="27" t="n"/>
+      <c r="L92" s="27" t="n"/>
       <c r="M92" s="20" t="n"/>
-      <c r="N92" s="55" t="n"/>
-      <c r="O92" s="54" t="n"/>
+      <c r="N92" s="27" t="n"/>
+      <c r="O92" s="26" t="n"/>
     </row>
     <row r="93" ht="8.1" customHeight="1" s="18">
-      <c r="B93" s="55" t="n"/>
-      <c r="C93" s="55" t="n"/>
+      <c r="B93" s="27" t="n"/>
+      <c r="C93" s="27" t="n"/>
       <c r="D93" s="22" t="n"/>
       <c r="E93" s="65" t="inlineStr">
         <is>
@@ -2177,17 +2177,17 @@
         </is>
       </c>
       <c r="F93" s="60" t="n"/>
-      <c r="H93" s="55" t="n"/>
-      <c r="I93" s="55" t="n"/>
-      <c r="K93" s="55" t="n"/>
-      <c r="L93" s="55" t="n"/>
+      <c r="H93" s="27" t="n"/>
+      <c r="I93" s="27" t="n"/>
+      <c r="K93" s="27" t="n"/>
+      <c r="L93" s="27" t="n"/>
       <c r="M93" s="20" t="n"/>
-      <c r="N93" s="55" t="n"/>
-      <c r="O93" s="54" t="n"/>
+      <c r="N93" s="27" t="n"/>
+      <c r="O93" s="26" t="n"/>
     </row>
     <row r="94" ht="8.1" customHeight="1" s="18">
-      <c r="B94" s="55" t="n"/>
-      <c r="C94" s="55" t="n"/>
+      <c r="B94" s="27" t="n"/>
+      <c r="C94" s="27" t="n"/>
       <c r="D94" s="19" t="n"/>
       <c r="E94" s="67" t="inlineStr">
         <is>
@@ -2195,13 +2195,13 @@
         </is>
       </c>
       <c r="F94" s="62" t="n"/>
-      <c r="H94" s="55" t="n"/>
-      <c r="I94" s="55" t="n"/>
-      <c r="K94" s="55" t="n"/>
-      <c r="L94" s="55" t="n"/>
+      <c r="H94" s="27" t="n"/>
+      <c r="I94" s="27" t="n"/>
+      <c r="K94" s="27" t="n"/>
+      <c r="L94" s="27" t="n"/>
       <c r="M94" s="20" t="n"/>
-      <c r="N94" s="55" t="n"/>
-      <c r="O94" s="54" t="n"/>
+      <c r="N94" s="27" t="n"/>
+      <c r="O94" s="26" t="n"/>
     </row>
     <row r="95" ht="8.1" customHeight="1" s="18">
       <c r="B95" s="65" t="inlineStr">
@@ -2210,15 +2210,15 @@
         </is>
       </c>
       <c r="C95" s="60" t="n"/>
-      <c r="E95" s="55" t="n"/>
-      <c r="F95" s="55" t="n"/>
-      <c r="H95" s="55" t="n"/>
-      <c r="I95" s="55" t="n"/>
-      <c r="K95" s="55" t="n"/>
-      <c r="L95" s="55" t="n"/>
+      <c r="E95" s="27" t="n"/>
+      <c r="F95" s="27" t="n"/>
+      <c r="H95" s="27" t="n"/>
+      <c r="I95" s="27" t="n"/>
+      <c r="K95" s="27" t="n"/>
+      <c r="L95" s="27" t="n"/>
       <c r="M95" s="20" t="n"/>
-      <c r="N95" s="55" t="n"/>
-      <c r="O95" s="54" t="n"/>
+      <c r="N95" s="27" t="n"/>
+      <c r="O95" s="26" t="n"/>
     </row>
     <row r="96" ht="8.1" customHeight="1" s="18">
       <c r="B96" s="67" t="inlineStr">
@@ -2227,38 +2227,38 @@
         </is>
       </c>
       <c r="C96" s="62" t="n"/>
-      <c r="E96" s="55" t="n"/>
-      <c r="F96" s="55" t="n"/>
-      <c r="H96" s="55" t="n"/>
-      <c r="I96" s="55" t="n"/>
-      <c r="K96" s="55" t="n"/>
-      <c r="L96" s="55" t="n"/>
+      <c r="E96" s="27" t="n"/>
+      <c r="F96" s="27" t="n"/>
+      <c r="H96" s="27" t="n"/>
+      <c r="I96" s="27" t="n"/>
+      <c r="K96" s="27" t="n"/>
+      <c r="L96" s="27" t="n"/>
       <c r="M96" s="20" t="n"/>
-      <c r="N96" s="56" t="n"/>
-      <c r="O96" s="57" t="n"/>
+      <c r="N96" s="28" t="n"/>
+      <c r="O96" s="29" t="n"/>
     </row>
     <row r="97" ht="8.1" customHeight="1" s="18">
-      <c r="B97" s="55" t="n"/>
-      <c r="C97" s="55" t="n"/>
-      <c r="E97" s="55" t="n"/>
-      <c r="F97" s="55" t="n"/>
-      <c r="H97" s="55" t="n"/>
-      <c r="I97" s="55" t="n"/>
-      <c r="K97" s="55" t="n"/>
-      <c r="L97" s="55" t="n"/>
+      <c r="B97" s="27" t="n"/>
+      <c r="C97" s="27" t="n"/>
+      <c r="E97" s="27" t="n"/>
+      <c r="F97" s="27" t="n"/>
+      <c r="H97" s="27" t="n"/>
+      <c r="I97" s="27" t="n"/>
+      <c r="K97" s="27" t="n"/>
+      <c r="L97" s="27" t="n"/>
       <c r="M97" s="22" t="n"/>
       <c r="N97" s="65" t="n"/>
       <c r="O97" s="60" t="n"/>
     </row>
     <row r="98" ht="8.1" customHeight="1" s="18">
-      <c r="B98" s="55" t="n"/>
-      <c r="C98" s="55" t="n"/>
-      <c r="E98" s="55" t="n"/>
-      <c r="F98" s="55" t="n"/>
-      <c r="H98" s="55" t="n"/>
-      <c r="I98" s="55" t="n"/>
-      <c r="K98" s="55" t="n"/>
-      <c r="L98" s="55" t="n"/>
+      <c r="B98" s="27" t="n"/>
+      <c r="C98" s="27" t="n"/>
+      <c r="E98" s="27" t="n"/>
+      <c r="F98" s="27" t="n"/>
+      <c r="H98" s="27" t="n"/>
+      <c r="I98" s="27" t="n"/>
+      <c r="K98" s="27" t="n"/>
+      <c r="L98" s="27" t="n"/>
       <c r="M98" s="20" t="n"/>
       <c r="N98" s="67" t="n"/>
       <c r="O98" s="62" t="n"/>
@@ -2270,12 +2270,12 @@
         </is>
       </c>
       <c r="C99" s="60" t="n"/>
-      <c r="E99" s="55" t="n"/>
-      <c r="F99" s="55" t="n"/>
-      <c r="H99" s="55" t="n"/>
-      <c r="I99" s="55" t="n"/>
-      <c r="K99" s="55" t="n"/>
-      <c r="L99" s="55" t="n"/>
+      <c r="E99" s="27" t="n"/>
+      <c r="F99" s="27" t="n"/>
+      <c r="H99" s="27" t="n"/>
+      <c r="I99" s="27" t="n"/>
+      <c r="K99" s="27" t="n"/>
+      <c r="L99" s="27" t="n"/>
       <c r="M99" s="20" t="n"/>
     </row>
     <row r="100" ht="8.1" customHeight="1" s="18">
@@ -2285,17 +2285,17 @@
         </is>
       </c>
       <c r="C100" s="62" t="n"/>
-      <c r="E100" s="55" t="n"/>
-      <c r="F100" s="55" t="n"/>
-      <c r="H100" s="55" t="n"/>
-      <c r="I100" s="55" t="n"/>
-      <c r="K100" s="55" t="n"/>
-      <c r="L100" s="55" t="n"/>
+      <c r="E100" s="27" t="n"/>
+      <c r="F100" s="27" t="n"/>
+      <c r="H100" s="27" t="n"/>
+      <c r="I100" s="27" t="n"/>
+      <c r="K100" s="27" t="n"/>
+      <c r="L100" s="27" t="n"/>
       <c r="M100" s="20" t="n"/>
     </row>
     <row r="101" ht="8.1" customHeight="1" s="18">
-      <c r="B101" s="55" t="n"/>
-      <c r="C101" s="55" t="n"/>
+      <c r="B101" s="27" t="n"/>
+      <c r="C101" s="27" t="n"/>
       <c r="D101" s="22" t="n"/>
       <c r="E101" s="59" t="inlineStr">
         <is>
@@ -2303,15 +2303,15 @@
         </is>
       </c>
       <c r="F101" s="60" t="n"/>
-      <c r="H101" s="55" t="n"/>
-      <c r="I101" s="55" t="n"/>
-      <c r="K101" s="55" t="n"/>
-      <c r="L101" s="55" t="n"/>
+      <c r="H101" s="27" t="n"/>
+      <c r="I101" s="27" t="n"/>
+      <c r="K101" s="27" t="n"/>
+      <c r="L101" s="27" t="n"/>
       <c r="M101" s="20" t="n"/>
     </row>
     <row r="102" ht="8.1" customHeight="1" s="18">
-      <c r="B102" s="55" t="n"/>
-      <c r="C102" s="55" t="n"/>
+      <c r="B102" s="27" t="n"/>
+      <c r="C102" s="27" t="n"/>
       <c r="D102" s="19" t="n"/>
       <c r="E102" s="61" t="inlineStr">
         <is>
@@ -2319,10 +2319,10 @@
         </is>
       </c>
       <c r="F102" s="62" t="n"/>
-      <c r="H102" s="55" t="n"/>
-      <c r="I102" s="55" t="n"/>
-      <c r="K102" s="55" t="n"/>
-      <c r="L102" s="55" t="n"/>
+      <c r="H102" s="27" t="n"/>
+      <c r="I102" s="27" t="n"/>
+      <c r="K102" s="27" t="n"/>
+      <c r="L102" s="27" t="n"/>
       <c r="M102" s="20" t="n"/>
     </row>
     <row r="103" ht="8.1" customHeight="1" s="18">
@@ -2332,49 +2332,49 @@
         </is>
       </c>
       <c r="C103" s="60" t="n"/>
-      <c r="E103" s="55" t="n"/>
-      <c r="F103" s="55" t="n"/>
+      <c r="E103" s="27" t="n"/>
+      <c r="F103" s="27" t="n"/>
       <c r="G103" s="20" t="n"/>
-      <c r="H103" s="55" t="n"/>
-      <c r="I103" s="55" t="n"/>
-      <c r="K103" s="55" t="n"/>
-      <c r="L103" s="55" t="n"/>
+      <c r="H103" s="27" t="n"/>
+      <c r="I103" s="27" t="n"/>
+      <c r="K103" s="27" t="n"/>
+      <c r="L103" s="27" t="n"/>
       <c r="M103" s="20" t="n"/>
     </row>
     <row r="104" ht="8.1" customHeight="1" s="18">
       <c r="B104" s="67" t="inlineStr"/>
       <c r="C104" s="62" t="n"/>
-      <c r="E104" s="55" t="n"/>
-      <c r="F104" s="55" t="n"/>
+      <c r="E104" s="27" t="n"/>
+      <c r="F104" s="27" t="n"/>
       <c r="G104" s="20" t="n"/>
-      <c r="H104" s="55" t="n"/>
-      <c r="I104" s="55" t="n"/>
-      <c r="K104" s="55" t="n"/>
-      <c r="L104" s="55" t="n"/>
+      <c r="H104" s="27" t="n"/>
+      <c r="I104" s="27" t="n"/>
+      <c r="K104" s="27" t="n"/>
+      <c r="L104" s="27" t="n"/>
       <c r="M104" s="20" t="n"/>
     </row>
     <row r="105" ht="8.1" customHeight="1" s="18">
-      <c r="B105" s="55" t="n"/>
-      <c r="C105" s="55" t="n"/>
-      <c r="E105" s="55" t="n"/>
-      <c r="F105" s="55" t="n"/>
+      <c r="B105" s="27" t="n"/>
+      <c r="C105" s="27" t="n"/>
+      <c r="E105" s="27" t="n"/>
+      <c r="F105" s="27" t="n"/>
       <c r="G105" s="22" t="n"/>
       <c r="H105" s="59" t="n"/>
       <c r="I105" s="60" t="n"/>
-      <c r="K105" s="55" t="n"/>
-      <c r="L105" s="55" t="n"/>
+      <c r="K105" s="27" t="n"/>
+      <c r="L105" s="27" t="n"/>
       <c r="M105" s="20" t="n"/>
     </row>
     <row r="106" ht="8.1" customHeight="1" s="18">
-      <c r="B106" s="55" t="n"/>
-      <c r="C106" s="55" t="n"/>
-      <c r="E106" s="55" t="n"/>
-      <c r="F106" s="55" t="n"/>
+      <c r="B106" s="27" t="n"/>
+      <c r="C106" s="27" t="n"/>
+      <c r="E106" s="27" t="n"/>
+      <c r="F106" s="27" t="n"/>
       <c r="G106" s="20" t="n"/>
       <c r="H106" s="61" t="n"/>
       <c r="I106" s="62" t="n"/>
-      <c r="K106" s="55" t="n"/>
-      <c r="L106" s="55" t="n"/>
+      <c r="K106" s="27" t="n"/>
+      <c r="L106" s="27" t="n"/>
       <c r="M106" s="20" t="n"/>
     </row>
     <row r="107" ht="8.1" customHeight="1" s="18">
@@ -2384,32 +2384,32 @@
         </is>
       </c>
       <c r="C107" s="60" t="n"/>
-      <c r="E107" s="55" t="n"/>
-      <c r="F107" s="55" t="n"/>
+      <c r="E107" s="27" t="n"/>
+      <c r="F107" s="27" t="n"/>
       <c r="G107" s="20" t="n"/>
-      <c r="H107" s="55" t="n"/>
-      <c r="I107" s="55" t="n"/>
+      <c r="H107" s="27" t="n"/>
+      <c r="I107" s="27" t="n"/>
       <c r="J107" s="20" t="n"/>
-      <c r="K107" s="55" t="n"/>
-      <c r="L107" s="55" t="n"/>
+      <c r="K107" s="27" t="n"/>
+      <c r="L107" s="27" t="n"/>
       <c r="M107" s="20" t="n"/>
     </row>
     <row r="108" ht="8.1" customHeight="1" s="18">
       <c r="B108" s="61" t="inlineStr"/>
       <c r="C108" s="62" t="n"/>
-      <c r="E108" s="55" t="n"/>
-      <c r="F108" s="55" t="n"/>
+      <c r="E108" s="27" t="n"/>
+      <c r="F108" s="27" t="n"/>
       <c r="G108" s="20" t="n"/>
-      <c r="H108" s="55" t="n"/>
-      <c r="I108" s="55" t="n"/>
+      <c r="H108" s="27" t="n"/>
+      <c r="I108" s="27" t="n"/>
       <c r="J108" s="20" t="n"/>
-      <c r="K108" s="55" t="n"/>
-      <c r="L108" s="55" t="n"/>
+      <c r="K108" s="27" t="n"/>
+      <c r="L108" s="27" t="n"/>
       <c r="M108" s="20" t="n"/>
     </row>
     <row r="109" ht="8.1" customHeight="1" s="18">
-      <c r="B109" s="55" t="n"/>
-      <c r="C109" s="55" t="n"/>
+      <c r="B109" s="27" t="n"/>
+      <c r="C109" s="27" t="n"/>
       <c r="D109" s="22" t="n"/>
       <c r="E109" s="65" t="inlineStr">
         <is>
@@ -2417,16 +2417,16 @@
         </is>
       </c>
       <c r="F109" s="60" t="n"/>
-      <c r="H109" s="55" t="n"/>
-      <c r="I109" s="55" t="n"/>
+      <c r="H109" s="27" t="n"/>
+      <c r="I109" s="27" t="n"/>
       <c r="J109" s="20" t="n"/>
-      <c r="K109" s="55" t="n"/>
-      <c r="L109" s="55" t="n"/>
+      <c r="K109" s="27" t="n"/>
+      <c r="L109" s="27" t="n"/>
       <c r="M109" s="20" t="n"/>
     </row>
     <row r="110" ht="8.1" customHeight="1" s="18">
-      <c r="B110" s="55" t="n"/>
-      <c r="C110" s="55" t="n"/>
+      <c r="B110" s="27" t="n"/>
+      <c r="C110" s="27" t="n"/>
       <c r="D110" s="19" t="n"/>
       <c r="E110" s="67" t="inlineStr">
         <is>
@@ -2434,11 +2434,11 @@
         </is>
       </c>
       <c r="F110" s="62" t="n"/>
-      <c r="H110" s="55" t="n"/>
-      <c r="I110" s="55" t="n"/>
+      <c r="H110" s="27" t="n"/>
+      <c r="I110" s="27" t="n"/>
       <c r="J110" s="20" t="n"/>
-      <c r="K110" s="55" t="n"/>
-      <c r="L110" s="55" t="n"/>
+      <c r="K110" s="27" t="n"/>
+      <c r="L110" s="27" t="n"/>
       <c r="M110" s="20" t="n"/>
     </row>
     <row r="111" ht="8.1" customHeight="1" s="18">
@@ -2448,13 +2448,13 @@
         </is>
       </c>
       <c r="C111" s="60" t="n"/>
-      <c r="E111" s="55" t="n"/>
-      <c r="F111" s="55" t="n"/>
-      <c r="H111" s="55" t="n"/>
-      <c r="I111" s="55" t="n"/>
+      <c r="E111" s="27" t="n"/>
+      <c r="F111" s="27" t="n"/>
+      <c r="H111" s="27" t="n"/>
+      <c r="I111" s="27" t="n"/>
       <c r="J111" s="20" t="n"/>
-      <c r="K111" s="55" t="n"/>
-      <c r="L111" s="55" t="n"/>
+      <c r="K111" s="27" t="n"/>
+      <c r="L111" s="27" t="n"/>
       <c r="M111" s="20" t="n"/>
     </row>
     <row r="112" ht="8.1" customHeight="1" s="18">
@@ -2464,39 +2464,39 @@
         </is>
       </c>
       <c r="C112" s="62" t="n"/>
-      <c r="E112" s="55" t="n"/>
-      <c r="F112" s="55" t="n"/>
-      <c r="H112" s="55" t="n"/>
-      <c r="I112" s="55" t="n"/>
+      <c r="E112" s="27" t="n"/>
+      <c r="F112" s="27" t="n"/>
+      <c r="H112" s="27" t="n"/>
+      <c r="I112" s="27" t="n"/>
       <c r="J112" s="20" t="n"/>
-      <c r="K112" s="55" t="n"/>
-      <c r="L112" s="55" t="n"/>
+      <c r="K112" s="27" t="n"/>
+      <c r="L112" s="27" t="n"/>
       <c r="M112" s="20" t="n"/>
     </row>
     <row r="113" ht="8.1" customHeight="1" s="18">
-      <c r="B113" s="55" t="n"/>
-      <c r="C113" s="55" t="n"/>
-      <c r="E113" s="55" t="n"/>
-      <c r="F113" s="55" t="n"/>
-      <c r="H113" s="55" t="n"/>
-      <c r="I113" s="55" t="n"/>
+      <c r="B113" s="27" t="n"/>
+      <c r="C113" s="27" t="n"/>
+      <c r="E113" s="27" t="n"/>
+      <c r="F113" s="27" t="n"/>
+      <c r="H113" s="27" t="n"/>
+      <c r="I113" s="27" t="n"/>
       <c r="J113" s="22" t="n"/>
       <c r="K113" s="65" t="n"/>
       <c r="L113" s="60" t="n"/>
-      <c r="N113" s="52" t="inlineStr">
+      <c r="N113" s="48" t="inlineStr">
         <is>
           <t>1st Place:</t>
         </is>
       </c>
-      <c r="P113" s="51" t="n"/>
+      <c r="P113" s="37" t="n"/>
     </row>
     <row r="114" ht="8.1" customHeight="1" s="18">
-      <c r="B114" s="55" t="n"/>
-      <c r="C114" s="55" t="n"/>
-      <c r="E114" s="55" t="n"/>
-      <c r="F114" s="55" t="n"/>
-      <c r="H114" s="55" t="n"/>
-      <c r="I114" s="55" t="n"/>
+      <c r="B114" s="27" t="n"/>
+      <c r="C114" s="27" t="n"/>
+      <c r="E114" s="27" t="n"/>
+      <c r="F114" s="27" t="n"/>
+      <c r="H114" s="27" t="n"/>
+      <c r="I114" s="27" t="n"/>
       <c r="J114" s="20" t="n"/>
       <c r="K114" s="67" t="n"/>
       <c r="L114" s="62" t="n"/>
@@ -2512,10 +2512,10 @@
         </is>
       </c>
       <c r="C115" s="60" t="n"/>
-      <c r="E115" s="55" t="n"/>
-      <c r="F115" s="55" t="n"/>
-      <c r="H115" s="55" t="n"/>
-      <c r="I115" s="55" t="n"/>
+      <c r="E115" s="27" t="n"/>
+      <c r="F115" s="27" t="n"/>
+      <c r="H115" s="27" t="n"/>
+      <c r="I115" s="27" t="n"/>
       <c r="J115" s="20" t="n"/>
       <c r="N115" s="10" t="n"/>
       <c r="O115" s="10" t="n"/>
@@ -2527,21 +2527,21 @@
         </is>
       </c>
       <c r="C116" s="62" t="n"/>
-      <c r="E116" s="55" t="n"/>
-      <c r="F116" s="55" t="n"/>
-      <c r="H116" s="55" t="n"/>
-      <c r="I116" s="55" t="n"/>
+      <c r="E116" s="27" t="n"/>
+      <c r="F116" s="27" t="n"/>
+      <c r="H116" s="27" t="n"/>
+      <c r="I116" s="27" t="n"/>
       <c r="J116" s="20" t="n"/>
-      <c r="N116" s="52" t="inlineStr">
+      <c r="N116" s="48" t="inlineStr">
         <is>
           <t>2nd Place:</t>
         </is>
       </c>
-      <c r="P116" s="51" t="n"/>
+      <c r="P116" s="37" t="n"/>
     </row>
     <row r="117" ht="8.1" customHeight="1" s="18">
-      <c r="B117" s="55" t="n"/>
-      <c r="C117" s="55" t="n"/>
+      <c r="B117" s="27" t="n"/>
+      <c r="C117" s="27" t="n"/>
       <c r="D117" s="22" t="n"/>
       <c r="E117" s="59" t="inlineStr">
         <is>
@@ -2549,8 +2549,8 @@
         </is>
       </c>
       <c r="F117" s="60" t="n"/>
-      <c r="H117" s="55" t="n"/>
-      <c r="I117" s="55" t="n"/>
+      <c r="H117" s="27" t="n"/>
+      <c r="I117" s="27" t="n"/>
       <c r="J117" s="20" t="n"/>
       <c r="P117" s="58" t="n"/>
       <c r="Q117" s="58" t="n"/>
@@ -2558,8 +2558,8 @@
       <c r="S117" s="58" t="n"/>
     </row>
     <row r="118" ht="8.1" customHeight="1" s="18">
-      <c r="B118" s="55" t="n"/>
-      <c r="C118" s="55" t="n"/>
+      <c r="B118" s="27" t="n"/>
+      <c r="C118" s="27" t="n"/>
       <c r="D118" s="19" t="n"/>
       <c r="E118" s="61" t="inlineStr">
         <is>
@@ -2567,8 +2567,8 @@
         </is>
       </c>
       <c r="F118" s="62" t="n"/>
-      <c r="H118" s="55" t="n"/>
-      <c r="I118" s="55" t="n"/>
+      <c r="H118" s="27" t="n"/>
+      <c r="I118" s="27" t="n"/>
       <c r="J118" s="20" t="n"/>
       <c r="N118" s="10" t="n"/>
       <c r="O118" s="10" t="n"/>
@@ -2580,27 +2580,27 @@
         </is>
       </c>
       <c r="C119" s="60" t="n"/>
-      <c r="E119" s="55" t="n"/>
-      <c r="F119" s="55" t="n"/>
+      <c r="E119" s="27" t="n"/>
+      <c r="F119" s="27" t="n"/>
       <c r="G119" s="20" t="n"/>
-      <c r="H119" s="55" t="n"/>
-      <c r="I119" s="55" t="n"/>
+      <c r="H119" s="27" t="n"/>
+      <c r="I119" s="27" t="n"/>
       <c r="J119" s="20" t="n"/>
-      <c r="N119" s="52" t="inlineStr">
+      <c r="N119" s="48" t="inlineStr">
         <is>
           <t>3rd Place:</t>
         </is>
       </c>
-      <c r="P119" s="51" t="n"/>
+      <c r="P119" s="37" t="n"/>
     </row>
     <row r="120" ht="8.1" customHeight="1" s="18">
       <c r="B120" s="67" t="inlineStr"/>
       <c r="C120" s="62" t="n"/>
-      <c r="E120" s="55" t="n"/>
-      <c r="F120" s="55" t="n"/>
+      <c r="E120" s="27" t="n"/>
+      <c r="F120" s="27" t="n"/>
       <c r="G120" s="20" t="n"/>
-      <c r="H120" s="55" t="n"/>
-      <c r="I120" s="55" t="n"/>
+      <c r="H120" s="27" t="n"/>
+      <c r="I120" s="27" t="n"/>
       <c r="J120" s="20" t="n"/>
       <c r="P120" s="58" t="n"/>
       <c r="Q120" s="58" t="n"/>
@@ -2608,10 +2608,10 @@
       <c r="S120" s="58" t="n"/>
     </row>
     <row r="121" ht="8.1" customHeight="1" s="18">
-      <c r="B121" s="55" t="n"/>
-      <c r="C121" s="55" t="n"/>
-      <c r="E121" s="55" t="n"/>
-      <c r="F121" s="55" t="n"/>
+      <c r="B121" s="27" t="n"/>
+      <c r="C121" s="27" t="n"/>
+      <c r="E121" s="27" t="n"/>
+      <c r="F121" s="27" t="n"/>
       <c r="G121" s="22" t="n"/>
       <c r="H121" s="65" t="n"/>
       <c r="I121" s="60" t="n"/>
@@ -2619,19 +2619,19 @@
       <c r="O121" s="10" t="n"/>
     </row>
     <row r="122" ht="8.1" customHeight="1" s="18">
-      <c r="B122" s="55" t="n"/>
-      <c r="C122" s="55" t="n"/>
-      <c r="E122" s="55" t="n"/>
-      <c r="F122" s="55" t="n"/>
+      <c r="B122" s="27" t="n"/>
+      <c r="C122" s="27" t="n"/>
+      <c r="E122" s="27" t="n"/>
+      <c r="F122" s="27" t="n"/>
       <c r="G122" s="20" t="n"/>
       <c r="H122" s="67" t="n"/>
       <c r="I122" s="62" t="n"/>
-      <c r="N122" s="52" t="inlineStr">
+      <c r="N122" s="48" t="inlineStr">
         <is>
           <t>3rd Place:</t>
         </is>
       </c>
-      <c r="P122" s="51" t="n"/>
+      <c r="P122" s="37" t="n"/>
     </row>
     <row r="123" ht="8.1" customHeight="1" s="18">
       <c r="B123" s="59" t="inlineStr">
@@ -2640,8 +2640,8 @@
         </is>
       </c>
       <c r="C123" s="60" t="n"/>
-      <c r="E123" s="55" t="n"/>
-      <c r="F123" s="55" t="n"/>
+      <c r="E123" s="27" t="n"/>
+      <c r="F123" s="27" t="n"/>
       <c r="G123" s="20" t="n"/>
       <c r="P123" s="58" t="n"/>
       <c r="Q123" s="58" t="n"/>
@@ -2655,20 +2655,20 @@
         </is>
       </c>
       <c r="C124" s="62" t="n"/>
-      <c r="E124" s="55" t="n"/>
-      <c r="F124" s="55" t="n"/>
+      <c r="E124" s="27" t="n"/>
+      <c r="F124" s="27" t="n"/>
       <c r="G124" s="20" t="n"/>
     </row>
     <row r="125" ht="8.1" customHeight="1" s="18">
-      <c r="B125" s="55" t="n"/>
-      <c r="C125" s="55" t="n"/>
+      <c r="B125" s="27" t="n"/>
+      <c r="C125" s="27" t="n"/>
       <c r="D125" s="22" t="n"/>
       <c r="E125" s="65" t="inlineStr"/>
       <c r="F125" s="60" t="n"/>
     </row>
     <row r="126" ht="8.1" customHeight="1" s="18">
-      <c r="B126" s="55" t="n"/>
-      <c r="C126" s="55" t="n"/>
+      <c r="B126" s="27" t="n"/>
+      <c r="C126" s="27" t="n"/>
       <c r="D126" s="19" t="n"/>
       <c r="E126" s="67" t="inlineStr"/>
       <c r="F126" s="62" t="n"/>
@@ -2770,6 +2770,125 @@
     <row r="207" ht="8.1" customHeight="1" s="18"/>
   </sheetData>
   <mergeCells count="143">
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="K18:L18"/>
+    <mergeCell ref="K49:L49"/>
+    <mergeCell ref="K50:L50"/>
+    <mergeCell ref="K6:Q9"/>
+    <mergeCell ref="B63:C63"/>
+    <mergeCell ref="B64:C64"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="E6:F6"/>
+    <mergeCell ref="E22:F22"/>
+    <mergeCell ref="E38:F38"/>
+    <mergeCell ref="E53:F53"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E14:F14"/>
+    <mergeCell ref="E30:F30"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="E46:F46"/>
+    <mergeCell ref="E61:F61"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="B52:C52"/>
+    <mergeCell ref="B55:C55"/>
+    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="B7:C7"/>
+    <mergeCell ref="B8:C8"/>
+    <mergeCell ref="B11:C11"/>
+    <mergeCell ref="B59:C59"/>
+    <mergeCell ref="B60:C60"/>
+    <mergeCell ref="B43:C43"/>
+    <mergeCell ref="B44:C44"/>
+    <mergeCell ref="B47:C47"/>
+    <mergeCell ref="B48:C48"/>
+    <mergeCell ref="B51:C51"/>
+    <mergeCell ref="B56:C56"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="H10:I10"/>
+    <mergeCell ref="H26:I26"/>
+    <mergeCell ref="H58:I58"/>
+    <mergeCell ref="H9:I9"/>
+    <mergeCell ref="H41:I41"/>
+    <mergeCell ref="H42:I42"/>
+    <mergeCell ref="H25:I25"/>
+    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B23:C23"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="E37:F37"/>
+    <mergeCell ref="E29:F29"/>
+    <mergeCell ref="E21:F21"/>
+    <mergeCell ref="E13:F13"/>
+    <mergeCell ref="B12:C12"/>
+    <mergeCell ref="B15:C15"/>
+    <mergeCell ref="B16:C16"/>
+    <mergeCell ref="B19:C19"/>
+    <mergeCell ref="B20:C20"/>
+    <mergeCell ref="N1:O2"/>
+    <mergeCell ref="B127:C127"/>
+    <mergeCell ref="B128:C128"/>
+    <mergeCell ref="P81:Q82"/>
+    <mergeCell ref="P49:Q50"/>
+    <mergeCell ref="P62:Q62"/>
+    <mergeCell ref="P63:Q63"/>
+    <mergeCell ref="P60:Q61"/>
+    <mergeCell ref="N113:O114"/>
+    <mergeCell ref="N116:O117"/>
+    <mergeCell ref="N119:O120"/>
+    <mergeCell ref="N122:O123"/>
+    <mergeCell ref="H122:I122"/>
+    <mergeCell ref="B123:C123"/>
+    <mergeCell ref="B124:C124"/>
+    <mergeCell ref="E125:F125"/>
+    <mergeCell ref="E126:F126"/>
+    <mergeCell ref="E118:F118"/>
+    <mergeCell ref="B119:C119"/>
+    <mergeCell ref="B120:C120"/>
+    <mergeCell ref="H121:I121"/>
+    <mergeCell ref="K113:L113"/>
+    <mergeCell ref="K114:L114"/>
+    <mergeCell ref="B115:C115"/>
+    <mergeCell ref="B116:C116"/>
+    <mergeCell ref="E117:F117"/>
+    <mergeCell ref="B108:C108"/>
+    <mergeCell ref="E109:F109"/>
+    <mergeCell ref="E110:F110"/>
+    <mergeCell ref="B111:C111"/>
+    <mergeCell ref="B112:C112"/>
+    <mergeCell ref="B103:C103"/>
+    <mergeCell ref="B104:C104"/>
+    <mergeCell ref="H105:I105"/>
+    <mergeCell ref="H106:I106"/>
+    <mergeCell ref="B107:C107"/>
+    <mergeCell ref="N98:O98"/>
+    <mergeCell ref="B99:C99"/>
+    <mergeCell ref="B100:C100"/>
+    <mergeCell ref="E101:F101"/>
+    <mergeCell ref="E102:F102"/>
+    <mergeCell ref="E94:F94"/>
+    <mergeCell ref="B95:C95"/>
+    <mergeCell ref="B96:C96"/>
+    <mergeCell ref="N97:O97"/>
+    <mergeCell ref="B76:C76"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="H89:I89"/>
+    <mergeCell ref="H90:I90"/>
+    <mergeCell ref="B91:C91"/>
+    <mergeCell ref="B92:C92"/>
+    <mergeCell ref="E93:F93"/>
+    <mergeCell ref="B84:C84"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="B87:C87"/>
+    <mergeCell ref="B88:C88"/>
     <mergeCell ref="K1:L2"/>
     <mergeCell ref="N33:O33"/>
     <mergeCell ref="N34:O34"/>
@@ -2794,125 +2913,6 @@
     <mergeCell ref="B83:C83"/>
     <mergeCell ref="H74:I74"/>
     <mergeCell ref="B75:C75"/>
-    <mergeCell ref="B76:C76"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="H89:I89"/>
-    <mergeCell ref="H90:I90"/>
-    <mergeCell ref="B91:C91"/>
-    <mergeCell ref="B92:C92"/>
-    <mergeCell ref="E93:F93"/>
-    <mergeCell ref="B84:C84"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="E86:F86"/>
-    <mergeCell ref="B87:C87"/>
-    <mergeCell ref="B88:C88"/>
-    <mergeCell ref="H105:I105"/>
-    <mergeCell ref="H106:I106"/>
-    <mergeCell ref="B107:C107"/>
-    <mergeCell ref="N98:O98"/>
-    <mergeCell ref="B99:C99"/>
-    <mergeCell ref="B100:C100"/>
-    <mergeCell ref="E101:F101"/>
-    <mergeCell ref="E102:F102"/>
-    <mergeCell ref="E94:F94"/>
-    <mergeCell ref="B95:C95"/>
-    <mergeCell ref="B96:C96"/>
-    <mergeCell ref="N97:O97"/>
-    <mergeCell ref="B116:C116"/>
-    <mergeCell ref="E117:F117"/>
-    <mergeCell ref="B108:C108"/>
-    <mergeCell ref="E109:F109"/>
-    <mergeCell ref="E110:F110"/>
-    <mergeCell ref="B111:C111"/>
-    <mergeCell ref="B112:C112"/>
-    <mergeCell ref="B103:C103"/>
-    <mergeCell ref="B104:C104"/>
-    <mergeCell ref="N1:O2"/>
-    <mergeCell ref="B127:C127"/>
-    <mergeCell ref="B128:C128"/>
-    <mergeCell ref="P81:Q82"/>
-    <mergeCell ref="P49:Q50"/>
-    <mergeCell ref="P62:Q62"/>
-    <mergeCell ref="P63:Q63"/>
-    <mergeCell ref="P60:Q61"/>
-    <mergeCell ref="N113:O114"/>
-    <mergeCell ref="N116:O117"/>
-    <mergeCell ref="N119:O120"/>
-    <mergeCell ref="N122:O123"/>
-    <mergeCell ref="H122:I122"/>
-    <mergeCell ref="B123:C123"/>
-    <mergeCell ref="B124:C124"/>
-    <mergeCell ref="E125:F125"/>
-    <mergeCell ref="E126:F126"/>
-    <mergeCell ref="E118:F118"/>
-    <mergeCell ref="B119:C119"/>
-    <mergeCell ref="B120:C120"/>
-    <mergeCell ref="H121:I121"/>
-    <mergeCell ref="K113:L113"/>
-    <mergeCell ref="K114:L114"/>
-    <mergeCell ref="B115:C115"/>
-    <mergeCell ref="H10:I10"/>
-    <mergeCell ref="H26:I26"/>
-    <mergeCell ref="H58:I58"/>
-    <mergeCell ref="H9:I9"/>
-    <mergeCell ref="H41:I41"/>
-    <mergeCell ref="H42:I42"/>
-    <mergeCell ref="H25:I25"/>
-    <mergeCell ref="H57:I57"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B23:C23"/>
-    <mergeCell ref="B24:C24"/>
-    <mergeCell ref="E37:F37"/>
-    <mergeCell ref="E29:F29"/>
-    <mergeCell ref="E21:F21"/>
-    <mergeCell ref="E13:F13"/>
-    <mergeCell ref="B12:C12"/>
-    <mergeCell ref="B15:C15"/>
-    <mergeCell ref="B16:C16"/>
-    <mergeCell ref="B19:C19"/>
-    <mergeCell ref="B20:C20"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="B7:C7"/>
-    <mergeCell ref="B8:C8"/>
-    <mergeCell ref="B11:C11"/>
-    <mergeCell ref="B59:C59"/>
-    <mergeCell ref="B60:C60"/>
-    <mergeCell ref="B43:C43"/>
-    <mergeCell ref="B44:C44"/>
-    <mergeCell ref="B47:C47"/>
-    <mergeCell ref="B48:C48"/>
-    <mergeCell ref="B51:C51"/>
-    <mergeCell ref="B56:C56"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="K18:L18"/>
-    <mergeCell ref="K49:L49"/>
-    <mergeCell ref="K50:L50"/>
-    <mergeCell ref="K6:Q9"/>
-    <mergeCell ref="B63:C63"/>
-    <mergeCell ref="B64:C64"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="E6:F6"/>
-    <mergeCell ref="E22:F22"/>
-    <mergeCell ref="E38:F38"/>
-    <mergeCell ref="E53:F53"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E14:F14"/>
-    <mergeCell ref="E30:F30"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="E46:F46"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="B52:C52"/>
-    <mergeCell ref="B55:C55"/>
-    <mergeCell ref="B27:C27"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B31:C31"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="landscape"/>

</xml_diff>